<commit_message>
Foi adicionada uma lista mais completa de user-agents.  Adicionada a função coletar_bullets_points, que coleta a descrição em tópicos do produto.  Adicionada a função coletar_imagem, que coleta o link da imagem principal do produto. Adicionada a função coletar_qtd_imagem, que percorre por cada thumbnail e retorna o valor total de imagens daquele produto. Adicionada a função coletar_qualidade_imagem, que veirifca a qualidade da imagem principal do produto (a mais importante para aumentar a relevância do anúncio na Amazon). A função coletar_dados_produtos foi ajustada, adicionando todas as funções criadas anteriormente.
</commit_message>
<xml_diff>
--- a/arquivo_convertido.xlsx
+++ b/arquivo_convertido.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,26 @@
       <c r="E1" s="1" t="inlineStr">
         <is>
           <t>qtd_avaliacao</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>bullets</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>imagem</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>qtd_imagem</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>qualidade_imagem</t>
         </is>
       </c>
     </row>
@@ -514,19 +534,313 @@
       <c r="E2" t="n">
         <v>1</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>['Portatil e fácil de carregar', 'Alta velocidade de transmissão', 'Compatibilidade']</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/31g-tls+1xL._AC_.jpg</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Meias Kids Selene 3 Pares Sortidos</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R$30,99</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ofereça conforto e estilo para os pequenos com as Meias Kids Selene. Perfeitas para o dia a dia, essas meias são ideais para garantir que as crianças estejam sempre aquecidas e bem vestidas, sem abrir mão da praticidade e do charme.
+Características Principais:
+Pacote com 3 Pares Sortidos: Cada pacote contém três pares de meias em cores e padrões variados, proporcionando opções versáteis para combinar com diferentes roupas e ocasiões.
+Conforto Superior: Feitas com materiais macios e respiráveis, as meias garantem um ajuste confortável e agradável durante todo o dia, evitando irritações e desconforto.
+Composição de Qualidade: Fabricadas com uma mistura de algodão e elastano, oferecem elasticidade e durabilidade, mantendo a forma e o ajuste perfeito após várias lavagens.
+Design Atraente: Disponíveis em uma variedade de cores e padrões divertidos, as meias adicionam um toque de diversão e estilo ao visual das crianças.
+Ajuste Perfeito: O elástico suave na parte superior ajuda a manter as meias no lugar sem apertar, proporcionando um ajuste seguro e confortável.
+Fácil Cuidados: Podem ser lavadas na máquina e secas ao ar livre, mantendo a praticidade para os pais e a durabilidade para os pequenos.
+As Meias Kids Selene são a escolha ideal para pais que buscam qualidade e estilo para seus filhos. Com a combinação perfeita de conforto, durabilidade e design, essas meias são um complemento essencial para o guarda-roupa das crianças.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Sem avaliação</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>['Bullet points não encontrados']</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61PCujaCXDL._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1060x722</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ring Light 6 Polegadas 14cm com Mini Tripe (Preto)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R$30,90</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Ring Light 6 Polegadas (14cm) com Mini Tripé! Ideal para criadores de conteúdo, maquiadores, youtubers e influenciadores, essa iluminação prática e eficiente é o segredo para resultados profissionais. Com seu design compacto e 3 opções de temperatura de cor (branca, neutra e quente), você terá o controle perfeito da luz, ajustando-a conforme o ambiente e o estilo de gravação. O mini tripé garante estabilidade e facilidade de uso em qualquer superfície, oferecendo ângulos ideais para selfies, gravações e videochamadas. Compacto, portátil e extremamente versátil, o Ring Light de 14cm é a escolha perfeita para destacar seus melhores momentos, melhorar a qualidade visual do seu conteúdo e proporcionar aquele brilho único que faz toda a diferença. Destaques: 3 modos de iluminação para ajuste perfeito; Mini tripé estável para qualquer superfície; Ideal para vídeos, fotos, lives e tutoriais; Compacto e leve, fácil de transportar.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Sem avaliação</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>['Versatilidade de Iluminação: Com três opções de temperatura de cor (branca, neutra e quente), o Ring Light permite que você ajuste a iluminação conforme o ambiente e o estilo de gravação, garantindo resultados sempre profissionais.', 'Portabilidade e Design Compacto: Seu tamanho reduzido e leveza tornam este ring light extremamente fácil de transportar, ideal para criadores de conteúdo em movimento, maquiadores e influenciadores que precisam de uma solução prática.', 'Mini Tripé Estável: O mini tripé proporciona estabilidade em qualquer superfície, permitindo ângulos ideais para selfies, gravações e videochamadas, sem comprometer a qualidade da imagem.', 'Ideal para Múltiplas Aplicações: Perfeito para vídeos, fotos, transmissões ao vivo e tutoriais, o Ring Light é uma ferramenta essencial para quem deseja elevar a qualidade visual do seu conteúdo.', 'Facilidade de Uso: A combinação de um design intuitivo com a funcionalidade do tripé torna este ring light fácil de usar, proporcionando uma experiência sem complicações para todos os criadores de conteúdo, independentemente do nível de experiência.']</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/516F0uDJazL._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1200x1133</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Biquíni Aviação Estampado Sem Bojo Conforto e Estilo</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R$44,99</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Transforme seu Verão com o Biquíni Aviação com Estampa Pimenta
+Prepare-se para brilhar neste verão com o Biquíni Aviação com Estampa Pimenta. Com um design vibrante e ousado, este biquíni é perfeito para quem deseja se destacar à beira da piscina ou na praia. A estampa de pimenta traz um toque de personalidade e modernidade, tornando cada momento ainda mais especial.
+Estampa Exclusiva: A estampa de pimenta não só adiciona um charme único e vibrante ao seu visual, mas também reflete seu estilo arrojado e confiante.
+Conforto Sem Bojo: A ausência de bojo garante um ajuste leve e confortável, ideal para dias ensolarados de diversão e relaxamento. Você pode se mover livremente, sem abrir mão da elegância.
+Design Estiloso: Com um corte que valoriza as curvas, este biquíni é ideal para quem busca um look ousado e contemporâneo. Combine-o com seus acessórios favoritos e esteja pronta para arrasar!
+Transforme suas experiências de verão em momentos inesquecíveis com o Biquíni Aviação. Sinta-se confiante, estilosa e confortável em qualquer ocasião!</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sem avaliação</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>['Bullet points não encontrados']</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61jwBveWy3L._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>797x1034</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Capa Protetora Defender Preta Para Galaxy Tab III 7 Otterbox (Preto)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R$28,89</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Proteja seu Galaxy Tab III 7 com a Capa Protetora Defender da Otterbox, projetada para oferecer máxima segurança e funcionalidade. Esta capa é ideal para quem busca proteção robusta sem abrir mão do estilo. Características: - Proteção Superior: A tecnologia de absorção de impactos proporciona defesa contra quedas, arranhões e impactos, garantindo que seu dispositivo permaneça em perfeito estado. - Design Ergonômico: Com um encaixe seguro e confortável, a capa facilita o manuseio, permitindo que você utilize seu tablet com facilidade. - Acesso Total: A Capa Defender mantém todas as portas e botões acessíveis, permitindo o uso total das funcionalidades do seu Galaxy Tab III 7, sem a necessidade de remover a capa. - Material de Alta Qualidade: Fabricada com materiais duráveis, resistentes à abrasão e ao desgaste, garantindo longa vida útil. - Instalação Simples: A capa é fácil de instalar e remover, permitindo que você troque de acessório conforme suas necessidades. Dimensões e Peso: - Compatível com Galaxy Tab III 7. - Peso leve, ideal para transporte. Cores Disponíveis: - Preto clássico, que combina com qualquer estilo. Cuidados e Manutenção: - Limpeza com pano úmido. - Evitar contato com produtos químicos agressivos. Garanta a proteção que seu Galaxy Tab III 7 merece com a Capa Protetora Defender Preta da Otterbox. Perfeita para uso diário, viagens ou qualquer situação em que seu tablet esteja exposto a riscos.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Sem avaliação</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>['Proteção em Camadas: A capa possui três camadas de proteção, incluindo uma camada interna de policarbonato rígido que absorve impactos e uma camada externa emborrachada que oferece resistência adicional contra quedas e arranhões.', 'Design Resistente: A capa é projetada para suportar ambientes desafiadores e testes rigorosos, protegendo o dispositivo de quedas de até 2 metros', 'Acesso Total: Apesar da proteção, a capa permite fácil acesso a todos os botões, portas e funcionalidades do tablet, incluindo câmera e conector de carregamento, sem precisar remover a capa.', 'Material e Dimensões: A capa é feita de policarbonato e silicone emborrachado, leve e projetada para se ajustar perfeitamente ao Galaxy Tab III 7".']</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/41Vc49XdKZL._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>498x1148</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Bermuda Masculina Térmica De Compressão Lupo I-Max</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R$120,30</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>A Bermuda Lupo AM Térmica I-Max em azul marinho é a escolha ideal para quem busca alto desempenho e conforto durante treinos intensos e atividades físicas. Feita com a tecnologia I-Max, ela oferece uma excelente compressão, proporcionando suporte muscular que melhora a performance e reduz a fadiga. Seu tecido térmico mantém a temperatura corporal estável, garantindo conforto em climas frios ou quentes.
+Características:
+Tecnologia I-Max: compressão que auxilia na circulação sanguínea e aumenta a resistência durante o exercício.
+Tecido térmico: mantém o corpo na temperatura ideal em qualquer condição climática.
+Elasticidade: ajuste perfeito ao corpo, permitindo total liberdade de movimento.
+Design anatômico: molda-se ao corpo com um caimento perfeito, valorizando a silhueta.
+Cor azul marinho: sofisticada e fácil de combinar com outras peças esportivas.
+Costuras flat: evitam atrito e irritações na pele, garantindo máximo conforto durante o uso prolongado.
+Respirabilidade: tecido que facilita a ventilação e evita o acúmulo de suor.
+Essa bermuda é a opção certa para quem procura qualidade, desempenho e estilo em uma única peça. Seja para correr, malhar ou praticar esportes ao ar livre, a Bermuda Lupo AM Térmica I-Max é a sua companheira ideal.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sem avaliação</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>['Bullet points não encontrados']</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51Gb00LBw2L._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>828x1013</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Película Protetora de Vidro para Tela de Celular, para Motorola E4, Transparente</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>R$19,09</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Proteção além da sua expectativa. As películas são compostas de um vidro temperado especial, não atrapalha o touch do seu smartphone, mas protege muito mais contra riscos, arranhões e impactos de menor grau sobre a tela do aparelho.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>4,3 de 5</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>['Proteção além da sua expectativa', 'As películas são compostas de um vidro temperado especial, não atrapalha o touch do seu smartphone', 'Protege muito mais contra riscos, arranhões e impactos de menor grau sobre a tela do aparelho', 'Para Motorola E4']</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61HJECjobtL._AC_SL1000_.jpg</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>790x812</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>Kit 2 Cuecas Boxer Mash Preto/Preto Listrado</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>R$52,90</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Eleve o conforto do seu dia a dia com o Kit Boxer Microfibra 2 Peças da Mash, ideal para quem busca qualidade e praticidade em roupas íntimas. Este conjunto é perfeito para uso diário, proporcionando o máximo de conforto e durabilidade.
 Características principais:
@@ -544,178 +858,6 @@
 O Kit Boxer Microfibra 2 Peças da Mash é a escolha perfeita para quem preza por qualidade, conforto e estilo no dia a dia!</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Sem avaliação</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Meias Kids Selene 3 Pares Sortidos</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R$30,99</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Ofereça conforto e estilo para os pequenos com as Meias Kids Selene. Perfeitas para o dia a dia, essas meias são ideais para garantir que as crianças estejam sempre aquecidas e bem vestidas, sem abrir mão da praticidade e do charme.
-Características Principais:
-Pacote com 3 Pares Sortidos: Cada pacote contém três pares de meias em cores e padrões variados, proporcionando opções versáteis para combinar com diferentes roupas e ocasiões.
-Conforto Superior: Feitas com materiais macios e respiráveis, as meias garantem um ajuste confortável e agradável durante todo o dia, evitando irritações e desconforto.
-Composição de Qualidade: Fabricadas com uma mistura de algodão e elastano, oferecem elasticidade e durabilidade, mantendo a forma e o ajuste perfeito após várias lavagens.
-Design Atraente: Disponíveis em uma variedade de cores e padrões divertidos, as meias adicionam um toque de diversão e estilo ao visual das crianças.
-Ajuste Perfeito: O elástico suave na parte superior ajuda a manter as meias no lugar sem apertar, proporcionando um ajuste seguro e confortável.
-Fácil Cuidados: Podem ser lavadas na máquina e secas ao ar livre, mantendo a praticidade para os pais e a durabilidade para os pequenos.
-As Meias Kids Selene são a escolha ideal para pais que buscam qualidade e estilo para seus filhos. Com a combinação perfeita de conforto, durabilidade e design, essas meias são um complemento essencial para o guarda-roupa das crianças.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Sem avaliação</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Bermuda Masculina Térmica De Compressão Lupo I-Max</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R$120,30</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>A Bermuda Lupo AM Térmica I-Max em azul marinho é a escolha ideal para quem busca alto desempenho e conforto durante treinos intensos e atividades físicas. Feita com a tecnologia I-Max, ela oferece uma excelente compressão, proporcionando suporte muscular que melhora a performance e reduz a fadiga. Seu tecido térmico mantém a temperatura corporal estável, garantindo conforto em climas frios ou quentes.
-Características:
-Tecnologia I-Max: compressão que auxilia na circulação sanguínea e aumenta a resistência durante o exercício.
-Tecido térmico: mantém o corpo na temperatura ideal em qualquer condição climática.
-Elasticidade: ajuste perfeito ao corpo, permitindo total liberdade de movimento.
-Design anatômico: molda-se ao corpo com um caimento perfeito, valorizando a silhueta.
-Cor azul marinho: sofisticada e fácil de combinar com outras peças esportivas.
-Costuras flat: evitam atrito e irritações na pele, garantindo máximo conforto durante o uso prolongado.
-Respirabilidade: tecido que facilita a ventilação e evita o acúmulo de suor.
-Essa bermuda é a opção certa para quem procura qualidade, desempenho e estilo em uma única peça. Seja para correr, malhar ou praticar esportes ao ar livre, a Bermuda Lupo AM Térmica I-Max é a sua companheira ideal.</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Sem avaliação</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Ring Light 6 Polegadas 14cm com Mini Tripe (Preto)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>R$30,90</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Ring Light 6 Polegadas (14cm) com Mini Tripé! Ideal para criadores de conteúdo, maquiadores, youtubers e influenciadores, essa iluminação prática e eficiente é o segredo para resultados profissionais. Com seu design compacto e 3 opções de temperatura de cor (branca, neutra e quente), você terá o controle perfeito da luz, ajustando-a conforme o ambiente e o estilo de gravação. O mini tripé garante estabilidade e facilidade de uso em qualquer superfície, oferecendo ângulos ideais para selfies, gravações e videochamadas. Compacto, portátil e extremamente versátil, o Ring Light de 14cm é a escolha perfeita para destacar seus melhores momentos, melhorar a qualidade visual do seu conteúdo e proporcionar aquele brilho único que faz toda a diferença. Destaques: 3 modos de iluminação para ajuste perfeito; Mini tripé estável para qualquer superfície; Ideal para vídeos, fotos, lives e tutoriais; Compacto e leve, fácil de transportar.</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Sem avaliação</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Biquíni Aviação Estampado Sem Bojo Conforto e Estilo</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>R$44,99</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Transforme seu Verão com o Biquíni Aviação com Estampa Pimenta
-Prepare-se para brilhar neste verão com o Biquíni Aviação com Estampa Pimenta. Com um design vibrante e ousado, este biquíni é perfeito para quem deseja se destacar à beira da piscina ou na praia. A estampa de pimenta traz um toque de personalidade e modernidade, tornando cada momento ainda mais especial.
-Estampa Exclusiva: A estampa de pimenta não só adiciona um charme único e vibrante ao seu visual, mas também reflete seu estilo arrojado e confiante.
-Conforto Sem Bojo: A ausência de bojo garante um ajuste leve e confortável, ideal para dias ensolarados de diversão e relaxamento. Você pode se mover livremente, sem abrir mão da elegância.
-Design Estiloso: Com um corte que valoriza as curvas, este biquíni é ideal para quem busca um look ousado e contemporâneo. Combine-o com seus acessórios favoritos e esteja pronta para arrasar!
-Transforme suas experiências de verão em momentos inesquecíveis com o Biquíni Aviação. Sinta-se confiante, estilosa e confortável em qualquer ocasião!</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Sem avaliação</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Película Protetora de Vidro para Tela de Celular, para Motorola E4, Transparente</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>R$19,09</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Proteção além da sua expectativa. As películas são compostas de um vidro temperado especial, não atrapalha o touch do seu smartphone, mas protege muito mais contra riscos, arranhões e impactos de menor grau sobre a tela do aparelho.</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>4,3 de 5</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Shorts Jeans Stillage Confortável com Barras Dobradas Estilo Casual</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>R$47,90</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Descubra o shorts perfeito para os dias quentes com o Shorts Jeans Stillage. Feito em jeans de alta qualidade, este modelo oferece o equilíbrio ideal entre conforto e estilo. Com barras dobradas que trazem um toque moderno e despojado, ele é a escolha ideal para compor looks casuais e frescos. Versátil, combina facilmente com blusas, camisetas ou regatas, sendo perfeito para passeios ou momentos descontraídos. Além disso, o corte ajustado valoriza a silhueta, proporcionando liberdade de movimento sem abrir mão do estilo.</t>
-        </is>
-      </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>Sem avaliação</t>
@@ -724,55 +866,109 @@
       <c r="E9" t="n">
         <v>0</v>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>['Bullet points não encontrados']</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51WYmEtPS1L._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>833x1137</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Capa Protetora Defender Preta Para Galaxy Tab III 7 Otterbox (Preto)</t>
+          <t>Capa Protetora Kicktok para Galaxy S8 Plus, Samsung, Capa Protetora para Celular, Transparente</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R$28,89</t>
+          <t>R$31,23</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Proteja seu Galaxy Tab III 7 com a Capa Protetora Defender da Otterbox, projetada para oferecer máxima segurança e funcionalidade. Esta capa é ideal para quem busca proteção robusta sem abrir mão do estilo. Características: - Proteção Superior: A tecnologia de absorção de impactos proporciona defesa contra quedas, arranhões e impactos, garantindo que seu dispositivo permaneça em perfeito estado. - Design Ergonômico: Com um encaixe seguro e confortável, a capa facilita o manuseio, permitindo que você utilize seu tablet com facilidade. - Acesso Total: A Capa Defender mantém todas as portas e botões acessíveis, permitindo o uso total das funcionalidades do seu Galaxy Tab III 7, sem a necessidade de remover a capa. - Material de Alta Qualidade: Fabricada com materiais duráveis, resistentes à abrasão e ao desgaste, garantindo longa vida útil. - Instalação Simples: A capa é fácil de instalar e remover, permitindo que você troque de acessório conforme suas necessidades. Dimensões e Peso: - Compatível com Galaxy Tab III 7. - Peso leve, ideal para transporte. Cores Disponíveis: - Preto clássico, que combina com qualquer estilo. Cuidados e Manutenção: - Limpeza com pano úmido. - Evitar contato com produtos químicos agressivos. Garanta a proteção que seu Galaxy Tab III 7 merece com a Capa Protetora Defender Preta da Otterbox. Perfeita para uso diário, viagens ou qualquer situação em que seu tablet esteja exposto a riscos.</t>
+          <t>A capa S8 kicktok protege o Galaxy S8 plus realçando o design do smartphone. A capa serve também como apoio permitindo uma posição confortável para visualização da tela ou para digitação além de permitir acesso rápido e fácil a todos os botões e conexões.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Sem avaliação</t>
+          <t>3,8 de 5</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>['Estilo e elegância', 'Proteção completa contra riscos e quedas', 'Suporte embutido para assistir a vídeos com as mãos livres', 'País de Origem: VN']</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51jZ4MDpKBL._AC_SL1499_.jpg</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>4</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>681x1443</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Capa Protetora Kicktok para Galaxy S8 Plus, Samsung, Capa Protetora para Celular, Transparente</t>
+          <t>Shorts Jeans Stillage Confortável com Barras Dobradas Estilo Casual</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R$31,23</t>
+          <t>R$47,90</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>A capa S8 kicktok protege o Galaxy S8 plus realçando o design do smartphone. A capa serve também como apoio permitindo uma posição confortável para visualização da tela ou para digitação além de permitir acesso rápido e fácil a todos os botões e conexões.</t>
+          <t>Descubra o shorts perfeito para os dias quentes com o Shorts Jeans Stillage. Feito em jeans de alta qualidade, este modelo oferece o equilíbrio ideal entre conforto e estilo. Com barras dobradas que trazem um toque moderno e despojado, ele é a escolha ideal para compor looks casuais e frescos. Versátil, combina facilmente com blusas, camisetas ou regatas, sendo perfeito para passeios ou momentos descontraídos. Além disso, o corte ajustado valoriza a silhueta, proporcionando liberdade de movimento sem abrir mão do estilo.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3,8 de 5</t>
+          <t>Sem avaliação</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>['Bullet points não encontrados']</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61mjwNm8C5L._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>1116x811</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -799,6 +995,24 @@
       <c r="E12" t="n">
         <v>20</v>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>['Adesivo de silicone', 'Fina e forte', 'Alta sensibilidade', 'A tela do seu aparelho sempre nova']</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71UPRh4y2oL._AC_SL1500_.jpg</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>724x1500</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -808,7 +1022,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R$48,99</t>
+          <t>R$45,41</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -824,55 +1038,109 @@
       <c r="E13" t="n">
         <v>3</v>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>['Para o uso de outros acessórios não precisa retirar a capa', 'Evite riscos e impactos que podem danificar seu aparelho.', 'Com acabamento refinado, dá maior aderência e segurança quando o aparelho está em suas mãos.', 'País de Origem: CN']</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/615aJ73lEBL._AC_SL1500_.jpg</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>638x1500</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Capa Protetora Cristal Case Transparente Moto E5, Motorola, Capa com Proteção Completa (Carcaça+Tela), Transparente</t>
+          <t>Carregador Veicular Hightech, Energizer, EZ-DCA2CUWH3I, Branca</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R$14,90</t>
+          <t>R$19,90</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Protege seu smartphone na parte traseira e laterais. com abertura para acessórios como carregadores e fones. Para o uso de outros acessórios não precisa retirar a capa. Evite riscos e impactos que podem danificar seu aparelho.</t>
+          <t>Carregue seus aparelhos enquanto está na rua ou na estrada. Com 3, 4 Amp potência de saída, este carregador Veicular Energizer com duas saídas USB, proporciona a carga rápida e segura de seus smartphones ou tablets.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>3,2 de 5</t>
+          <t>4,5 de 5</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>['Carregue dois aparelhos simultaneamente', 'Obs: Não acompanha cabo USB', 'Design elegante']</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61t5kdNN+3L._AC_SL1500_.jpg</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>1160x1248</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Carregador Veicular Hightech, Energizer, EZ-DCA2CUWH3I, Branca</t>
+          <t>Capa Protetora Cristal Case Transparente Moto E5, Motorola, Capa com Proteção Completa (Carcaça+Tela), Transparente</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R$19,90</t>
+          <t>R$14,90</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Carregue seus aparelhos enquanto está na rua ou na estrada. Com 3, 4 Amp potência de saída, este carregador Veicular Energizer com duas saídas USB, proporciona a carga rápida e segura de seus smartphones ou tablets.</t>
+          <t>Protege seu smartphone na parte traseira e laterais. com abertura para acessórios como carregadores e fones. Para o uso de outros acessórios não precisa retirar a capa. Evite riscos e impactos que podem danificar seu aparelho.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>4,5 de 5</t>
+          <t>3,2 de 5</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>11</v>
+        <v>33</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>['Protege seu smartphone na parte traseira e laterais. com abertura para acessórios como carregadores e fones', 'Para o uso de outros acessórios não precisa retirar a capa', 'Evite riscos e impactos que podem danificar seu aparelho', 'País de Origem: CN']</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/611KhH7BtTL._AC_SL1500_.jpg</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>697x1433</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -899,6 +1167,24 @@
       <c r="E16" t="n">
         <v>0</v>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>['Alta Resolução: Suporta resoluções de até 4K (2160p), proporcionando imagens nítidas e detalhadas, ideal para gamers e profissionais que exigem qualidade visual superior.', 'Blindagem Reforçada: A blindagem avançada do cabo protege contra interferências eletromagnéticas, minimizando perda de sinal e garantindo uma conexão de alta qualidade.', 'Conectores Banhados a Ouro: Os conectores banhados a ouro garantem uma excelente condutividade e resistência à corrosão, assegurando uma transmissão de sinal mais estável e confiável.', 'Trava de Segurança: Equipado com uma trava de segurança, o cabo assegura uma conexão firme e confiável, evitando desconexões acidentais durante o uso.', 'Comprimento Ideal: Com 1,8 metros de comprimento, o cabo oferece flexibilidade e conveniência para conectar dispositivos em diferentes configurações sem comprometer a qualidade do sinal.']</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51-3+Xs2w-L._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>1200x1091</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -924,6 +1210,24 @@
       <c r="E17" t="n">
         <v>0</v>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>['Eficiência de Carregamento: Com potência de 15W, o carregador oferece carregamento rápido e eficiente para uma variedade de dispositivos, incluindo smartphones e tablets.', 'Portabilidade e Design Compacto: O design leve e discreto facilita o transporte em bolsas e mochilas, tornando-o ideal para quem está sempre em movimento.', 'Compatibilidade Universal: A porta USB-A permite a conexão com uma ampla gama de dispositivos, garantindo flexibilidade no carregamento.', 'Segurança Avançada: Equipado com proteção contra superaquecimento, sobrecarga e curtos-circuitos, assegura um uso seguro para os dispositivos.', 'Compatibilidade Global: Funciona em tensões de 100-240V, sendo ideal para viajantes que necessitam de um carregador confiável em diferentes regiões do mundo.']</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/41ybhWt-6iL._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>595x1185</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -949,6 +1253,24 @@
       <c r="E18" t="n">
         <v>0</v>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>['Com Design Limpo E Moderno, Trazendo Requinte E Sofisticação Para A Decoração De Seu Bar', 'Um Lindo Presente Para Homens Modernos Que Gostam De Preparar Seus Dinks Ou Receber Seus Convidados Com Elegncia', 'Em Aço Inox Polido, Prática De Limpar E Durável', 'País de Origem: CN']</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51n-vWG4HIL._AC_SL1000_.jpg</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>5</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>611x893</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -973,6 +1295,24 @@
       </c>
       <c r="E19" t="n">
         <v>2</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>['Ideal para limpar e tirar o pó na sala no quarto ou no seu escritório', 'Dobrável em aço e plástico com 45 cm', 'Material pp e aço inox', 'Fabricado com muito cuidado e atenção aos detalhes']</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/41n99saqHAL._AC_SL1000_.jpg</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>410x362</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tratamento para verificar a quantidade de caracter do titulo, a qualidade da imagem, a quantidade de imagem, se possui vídeo ou não. Salva as informações em um dataframe.
</commit_message>
<xml_diff>
--- a/arquivo_convertido.xlsx
+++ b/arquivo_convertido.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,37 +446,57 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>link</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>descricao</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>avaliacao</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>qtd_avaliacao</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>bullets</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>imagem</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>qtd_imagem</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>qualidade_imagem</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>video</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>nome_categoria</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>link_categoria</t>
         </is>
       </c>
     </row>
@@ -492,6 +512,11 @@
         </is>
       </c>
       <c r="C2" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Portas-Leitor-Cartao-Memoria-7portas/dp/B0DGGW72LL/ref=sr_1_1?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-1&amp;xpid=tqkuqdh5H_SQg</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>Características
 - HUB + Leitor de cartão universal
@@ -526,226 +551,59 @@
 - RS MMC-Speed/RS MMC-Max/MMC Pro/MMC Mobile/MMC/ Mobile-Pro</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>5 de 5</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>['Portatil e fácil de carregar', 'Alta velocidade de transmissão', 'Compatibilidade']</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>https://m.media-amazon.com/images/I/31g-tls+1xL._AC_.jpg</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>1</v>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Hubs USB</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Hubs-USB/b/ref=dp_bc_3?ie=UTF8&amp;node=23884302011</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Meias Kids Selene 3 Pares Sortidos</t>
+          <t>Bermuda Masculina Térmica De Compressão Lupo I-Max</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$30,99</t>
+          <t>R$120,30</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ofereça conforto e estilo para os pequenos com as Meias Kids Selene. Perfeitas para o dia a dia, essas meias são ideais para garantir que as crianças estejam sempre aquecidas e bem vestidas, sem abrir mão da praticidade e do charme.
-Características Principais:
-Pacote com 3 Pares Sortidos: Cada pacote contém três pares de meias em cores e padrões variados, proporcionando opções versáteis para combinar com diferentes roupas e ocasiões.
-Conforto Superior: Feitas com materiais macios e respiráveis, as meias garantem um ajuste confortável e agradável durante todo o dia, evitando irritações e desconforto.
-Composição de Qualidade: Fabricadas com uma mistura de algodão e elastano, oferecem elasticidade e durabilidade, mantendo a forma e o ajuste perfeito após várias lavagens.
-Design Atraente: Disponíveis em uma variedade de cores e padrões divertidos, as meias adicionam um toque de diversão e estilo ao visual das crianças.
-Ajuste Perfeito: O elástico suave na parte superior ajuda a manter as meias no lugar sem apertar, proporcionando um ajuste seguro e confortável.
-Fácil Cuidados: Podem ser lavadas na máquina e secas ao ar livre, mantendo a praticidade para os pais e a durabilidade para os pequenos.
-As Meias Kids Selene são a escolha ideal para pais que buscam qualidade e estilo para seus filhos. Com a combinação perfeita de conforto, durabilidade e design, essas meias são um complemento essencial para o guarda-roupa das crianças.</t>
+          <t>https://www.amazon.com.br/Bermuda-Masculina-T%C3%A9rmica-Compress%C3%A3o-I-Max/dp/B0DGQTCMC5/ref=sr_1_2?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-2&amp;ufe=app_do%3Aamzn1.fos.a492fd4a-f54d-4e8d-8c31-35e0a04ce61e&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
-        <is>
-          <t>Sem avaliação</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>['Bullet points não encontrados']</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>https://m.media-amazon.com/images/I/61PCujaCXDL._AC_SL1200_.jpg</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>1060x722</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Ring Light 6 Polegadas 14cm com Mini Tripe (Preto)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R$30,90</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Ring Light 6 Polegadas (14cm) com Mini Tripé! Ideal para criadores de conteúdo, maquiadores, youtubers e influenciadores, essa iluminação prática e eficiente é o segredo para resultados profissionais. Com seu design compacto e 3 opções de temperatura de cor (branca, neutra e quente), você terá o controle perfeito da luz, ajustando-a conforme o ambiente e o estilo de gravação. O mini tripé garante estabilidade e facilidade de uso em qualquer superfície, oferecendo ângulos ideais para selfies, gravações e videochamadas. Compacto, portátil e extremamente versátil, o Ring Light de 14cm é a escolha perfeita para destacar seus melhores momentos, melhorar a qualidade visual do seu conteúdo e proporcionar aquele brilho único que faz toda a diferença. Destaques: 3 modos de iluminação para ajuste perfeito; Mini tripé estável para qualquer superfície; Ideal para vídeos, fotos, lives e tutoriais; Compacto e leve, fácil de transportar.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Sem avaliação</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>['Versatilidade de Iluminação: Com três opções de temperatura de cor (branca, neutra e quente), o Ring Light permite que você ajuste a iluminação conforme o ambiente e o estilo de gravação, garantindo resultados sempre profissionais.', 'Portabilidade e Design Compacto: Seu tamanho reduzido e leveza tornam este ring light extremamente fácil de transportar, ideal para criadores de conteúdo em movimento, maquiadores e influenciadores que precisam de uma solução prática.', 'Mini Tripé Estável: O mini tripé proporciona estabilidade em qualquer superfície, permitindo ângulos ideais para selfies, gravações e videochamadas, sem comprometer a qualidade da imagem.', 'Ideal para Múltiplas Aplicações: Perfeito para vídeos, fotos, transmissões ao vivo e tutoriais, o Ring Light é uma ferramenta essencial para quem deseja elevar a qualidade visual do seu conteúdo.', 'Facilidade de Uso: A combinação de um design intuitivo com a funcionalidade do tripé torna este ring light fácil de usar, proporcionando uma experiência sem complicações para todos os criadores de conteúdo, independentemente do nível de experiência.']</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>https://m.media-amazon.com/images/I/516F0uDJazL._AC_SL1200_.jpg</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>1200x1133</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Biquíni Aviação Estampado Sem Bojo Conforto e Estilo</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R$44,99</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Transforme seu Verão com o Biquíni Aviação com Estampa Pimenta
-Prepare-se para brilhar neste verão com o Biquíni Aviação com Estampa Pimenta. Com um design vibrante e ousado, este biquíni é perfeito para quem deseja se destacar à beira da piscina ou na praia. A estampa de pimenta traz um toque de personalidade e modernidade, tornando cada momento ainda mais especial.
-Estampa Exclusiva: A estampa de pimenta não só adiciona um charme único e vibrante ao seu visual, mas também reflete seu estilo arrojado e confiante.
-Conforto Sem Bojo: A ausência de bojo garante um ajuste leve e confortável, ideal para dias ensolarados de diversão e relaxamento. Você pode se mover livremente, sem abrir mão da elegância.
-Design Estiloso: Com um corte que valoriza as curvas, este biquíni é ideal para quem busca um look ousado e contemporâneo. Combine-o com seus acessórios favoritos e esteja pronta para arrasar!
-Transforme suas experiências de verão em momentos inesquecíveis com o Biquíni Aviação. Sinta-se confiante, estilosa e confortável em qualquer ocasião!</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Sem avaliação</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>['Bullet points não encontrados']</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>https://m.media-amazon.com/images/I/61jwBveWy3L._AC_SL1200_.jpg</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>3</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>797x1034</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Capa Protetora Defender Preta Para Galaxy Tab III 7 Otterbox (Preto)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>R$28,89</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Proteja seu Galaxy Tab III 7 com a Capa Protetora Defender da Otterbox, projetada para oferecer máxima segurança e funcionalidade. Esta capa é ideal para quem busca proteção robusta sem abrir mão do estilo. Características: - Proteção Superior: A tecnologia de absorção de impactos proporciona defesa contra quedas, arranhões e impactos, garantindo que seu dispositivo permaneça em perfeito estado. - Design Ergonômico: Com um encaixe seguro e confortável, a capa facilita o manuseio, permitindo que você utilize seu tablet com facilidade. - Acesso Total: A Capa Defender mantém todas as portas e botões acessíveis, permitindo o uso total das funcionalidades do seu Galaxy Tab III 7, sem a necessidade de remover a capa. - Material de Alta Qualidade: Fabricada com materiais duráveis, resistentes à abrasão e ao desgaste, garantindo longa vida útil. - Instalação Simples: A capa é fácil de instalar e remover, permitindo que você troque de acessório conforme suas necessidades. Dimensões e Peso: - Compatível com Galaxy Tab III 7. - Peso leve, ideal para transporte. Cores Disponíveis: - Preto clássico, que combina com qualquer estilo. Cuidados e Manutenção: - Limpeza com pano úmido. - Evitar contato com produtos químicos agressivos. Garanta a proteção que seu Galaxy Tab III 7 merece com a Capa Protetora Defender Preta da Otterbox. Perfeita para uso diário, viagens ou qualquer situação em que seu tablet esteja exposto a riscos.</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Sem avaliação</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>['Proteção em Camadas: A capa possui três camadas de proteção, incluindo uma camada interna de policarbonato rígido que absorve impactos e uma camada externa emborrachada que oferece resistência adicional contra quedas e arranhões.', 'Design Resistente: A capa é projetada para suportar ambientes desafiadores e testes rigorosos, protegendo o dispositivo de quedas de até 2 metros', 'Acesso Total: Apesar da proteção, a capa permite fácil acesso a todos os botões, portas e funcionalidades do tablet, incluindo câmera e conector de carregamento, sem precisar remover a capa.', 'Material e Dimensões: A capa é feita de policarbonato e silicone emborrachado, leve e projetada para se ajustar perfeitamente ao Galaxy Tab III 7".']</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>https://m.media-amazon.com/images/I/41Vc49XdKZL._AC_SL1200_.jpg</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>498x1148</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Bermuda Masculina Térmica De Compressão Lupo I-Max</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>R$120,30</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
         <is>
           <t>A Bermuda Lupo AM Térmica I-Max em azul marinho é a escolha ideal para quem busca alto desempenho e conforto durante treinos intensos e atividades físicas. Feita com a tecnologia I-Max, ela oferece uma excelente compressão, proporcionando suporte muscular que melhora a performance e reduz a fadiga. Seu tecido térmico mantém a temperatura corporal estável, garantindo conforto em climas frios ou quentes.
 Características:
@@ -759,88 +617,129 @@
 Essa bermuda é a opção certa para quem procura qualidade, desempenho e estilo em uma única peça. Seja para correr, malhar ou praticar esportes ao ar livre, a Bermuda Lupo AM Térmica I-Max é a sua companheira ideal.</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Sem avaliação</t>
         </is>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>['Bullet points não encontrados']</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>['Elasticidade', 'Design anatômico', 'Respirabilidade', 'Tecido térmico']</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>https://m.media-amazon.com/images/I/51Gb00LBw2L._AC_SL1200_.jpg</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="I3" t="n">
         <v>1</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>828x1013</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Película Protetora de Vidro para Tela de Celular, para Motorola E4, Transparente</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>R$19,09</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Proteção além da sua expectativa. As películas são compostas de um vidro temperado especial, não atrapalha o touch do seu smartphone, mas protege muito mais contra riscos, arranhões e impactos de menor grau sobre a tela do aparelho.</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>4,3 de 5</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>31</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>['Proteção além da sua expectativa', 'As películas são compostas de um vidro temperado especial, não atrapalha o touch do seu smartphone', 'Protege muito mais contra riscos, arranhões e impactos de menor grau sobre a tela do aparelho', 'Para Motorola E4']</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>https://m.media-amazon.com/images/I/61HJECjobtL._AC_SL1000_.jpg</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>790x812</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Shorts e Bermudas</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=17682478011</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Biquíni Aviação Estampado Sem Bojo Conforto e Estilo</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R$44,99</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Biqu%C3%ADni-Avia%C3%A7%C3%A3o-Estampado-Conforto-Estilo/dp/B0DKQY7HWC/ref=sr_1_3?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-3&amp;ufe=app_do%3Aamzn1.fos.6d798eae-cadf-45de-946a-f477d47705b9&amp;xpid=tqkuqdh5H_SQg</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Transforme seu Verão com o Biquíni Aviação com Estampa Pimenta
+Prepare-se para brilhar neste verão com o Biquíni Aviação com Estampa Pimenta. Com um design vibrante e ousado, este biquíni é perfeito para quem deseja se destacar à beira da piscina ou na praia. A estampa de pimenta traz um toque de personalidade e modernidade, tornando cada momento ainda mais especial.
+Estampa Exclusiva: A estampa de pimenta não só adiciona um charme único e vibrante ao seu visual, mas também reflete seu estilo arrojado e confiante.
+Conforto Sem Bojo: A ausência de bojo garante um ajuste leve e confortável, ideal para dias ensolarados de diversão e relaxamento. Você pode se mover livremente, sem abrir mão da elegância.
+Design Estiloso: Com um corte que valoriza as curvas, este biquíni é ideal para quem busca um look ousado e contemporâneo. Combine-o com seus acessórios favoritos e esteja pronta para arrasar!
+Transforme suas experiências de verão em momentos inesquecíveis com o Biquíni Aviação. Sinta-se confiante, estilosa e confortável em qualquer ocasião!</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Sem avaliação</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>['Detalhes da estampa de pimenta e seu charme único', 'Conforto durante atividades', 'Valoriza as curvas e complementa o visual', 'Design Vibrante e Ousado']</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61jwBveWy3L._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>797x1034</t>
+        </is>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Conjuntos</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_6?ie=UTF8&amp;node=17682696011</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Kit 2 Cuecas Boxer Mash Preto/Preto Listrado</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>R$52,90</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Cuecas-Boxer-Mash-Preto-Listrado/dp/B0DGXZJ3TZ/ref=sr_1_4?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-4&amp;ufe=app_do%3Aamzn1.fos.6d798eae-cadf-45de-946a-f477d47705b9&amp;xpid=tqkuqdh5H_SQg</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>Eleve o conforto do seu dia a dia com o Kit Boxer Microfibra 2 Peças da Mash, ideal para quem busca qualidade e praticidade em roupas íntimas. Este conjunto é perfeito para uso diário, proporcionando o máximo de conforto e durabilidade.
 Características principais:
@@ -858,460 +757,832 @@
 O Kit Boxer Microfibra 2 Peças da Mash é a escolha perfeita para quem preza por qualidade, conforto e estilo no dia a dia!</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Sem avaliação</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>['Modelagem anatômica', 'Cintura elástica', 'Sem costura lateral', 'Respirabilidade', 'Kit com 2 peças']</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51WYmEtPS1L._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>833x1137</t>
+        </is>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Cuecas Samba-Canção</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=17682497011</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Capa Protetora Defender Preta Para Galaxy Tab III 7 Otterbox (Preto)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R$28,89</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Protetora-Defender-Preta-Galaxy-Otterbox/dp/B07QYV9KGQ/ref=sr_1_5?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-5&amp;xpid=tqkuqdh5H_SQg</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Proteja seu Galaxy Tab III 7 com a Capa Protetora Defender da Otterbox, projetada para oferecer máxima segurança e funcionalidade. Esta capa é ideal para quem busca proteção robusta sem abrir mão do estilo. Características: - Proteção Superior: A tecnologia de absorção de impactos proporciona defesa contra quedas, arranhões e impactos, garantindo que seu dispositivo permaneça em perfeito estado. - Design Ergonômico: Com um encaixe seguro e confortável, a capa facilita o manuseio, permitindo que você utilize seu tablet com facilidade. - Acesso Total: A Capa Defender mantém todas as portas e botões acessíveis, permitindo o uso total das funcionalidades do seu Galaxy Tab III 7, sem a necessidade de remover a capa. - Material de Alta Qualidade: Fabricada com materiais duráveis, resistentes à abrasão e ao desgaste, garantindo longa vida útil. - Instalação Simples: A capa é fácil de instalar e remover, permitindo que você troque de acessório conforme suas necessidades. Dimensões e Peso: - Compatível com Galaxy Tab III 7. - Peso leve, ideal para transporte. Cores Disponíveis: - Preto clássico, que combina com qualquer estilo. Cuidados e Manutenção: - Limpeza com pano úmido. - Evitar contato com produtos químicos agressivos. Garanta a proteção que seu Galaxy Tab III 7 merece com a Capa Protetora Defender Preta da Otterbox. Perfeita para uso diário, viagens ou qualquer situação em que seu tablet esteja exposto a riscos.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Sem avaliação</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>['Proteção em Camadas: A capa possui três camadas de proteção, incluindo uma camada interna de policarbonato rígido que absorve impactos e uma camada externa emborrachada que oferece resistência adicional contra quedas e arranhões.', 'Design Resistente: A capa é projetada para suportar ambientes desafiadores e testes rigorosos, protegendo o dispositivo de quedas de até 2 metros', 'Acesso Total: Apesar da proteção, a capa permite fácil acesso a todos os botões, portas e funcionalidades do tablet, incluindo câmera e conector de carregamento, sem precisar remover a capa.', 'Material e Dimensões: A capa é feita de policarbonato e silicone emborrachado, leve e projetada para se ajustar perfeitamente ao Galaxy Tab III 7".']</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/41Vc49XdKZL._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>498x1148</t>
+        </is>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Capas, Bolsas e Estojos</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_4?ie=UTF8&amp;node=16364864011</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Cabo Displayport 4k Blindado Macho X Macho 1,8m 1.1 E 1.2 (preto)</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R$31,90</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Cabo-Displayport-Blindado-Macho-preto/dp/B0DKPHT6SJ/ref=sr_1_6?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-6&amp;xpid=tqkuqdh5H_SQg</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>O Cabo DisplayPort 4K Blindado de 1,8 metros oferece qualidade de transmissão superior para quem busca desempenho e durabilidade. Com conectores banhados a ouro e blindagem reforçada, ele proporciona máxima proteção contra interferências e uma conexão estável. Ideal para quem exige alta definição em resoluções de até 4K, este cabo é perfeito para conectar notebooks, tablets, TVs, monitores e projetores com suporte DisplayPort. Características do Produto: Marca: F3 Modelo: JC-DP1.8 Resolução Suportada: 480i, 576i/p, 720i/p, 1080i/p, até 2160p (4K) Conectores: 2 x DisplayPort (Macho) com conectores banhados a ouro Padrões Compatíveis: DisplayPort 1.1 e 1.2 Comprimento do Cabo: 1,8 metro Cor: Preto Com trava de segurança, garantindo uma conexão firme e confiável. Garantia do vendedor: 90 dias</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Sem avaliação</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>['Alta Resolução: Suporta resoluções de até 4K (2160p), proporcionando imagens nítidas e detalhadas, ideal para gamers e profissionais que exigem qualidade visual superior.', 'Blindagem Reforçada: A blindagem avançada do cabo protege contra interferências eletromagnéticas, minimizando perda de sinal e garantindo uma conexão de alta qualidade.', 'Conectores Banhados a Ouro: Os conectores banhados a ouro garantem uma excelente condutividade e resistência à corrosão, assegurando uma transmissão de sinal mais estável e confiável.', 'Trava de Segurança: Equipado com uma trava de segurança, o cabo assegura uma conexão firme e confiável, evitando desconexões acidentais durante o uso.', 'Comprimento Ideal: Com 1,8 metros de comprimento, o cabo oferece flexibilidade e conveniência para conectar dispositivos em diferentes configurações sem comprometer a qualidade do sinal.']</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51-3+Xs2w-L._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>1200x1091</t>
+        </is>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Cabos DisplayPort</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16364884011</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Shorts Jeans Stillage Confortável com Barras Dobradas Estilo Casual</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>R$47,90</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Shorts-Stillage-Confort%C3%A1vel-Barras-Dobradas/dp/B0DGXZDBPY/ref=sr_1_7?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-7&amp;ufe=app_do%3Aamzn1.fos.6d798eae-cadf-45de-946a-f477d47705b9&amp;xpid=tqkuqdh5H_SQg</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Descubra o shorts perfeito para os dias quentes com o Shorts Jeans Stillage. Feito em jeans de alta qualidade, este modelo oferece o equilíbrio ideal entre conforto e estilo. Com barras dobradas que trazem um toque moderno e despojado, ele é a escolha ideal para compor looks casuais e frescos. Versátil, combina facilmente com blusas, camisetas ou regatas, sendo perfeito para passeios ou momentos descontraídos. Além disso, o corte ajustado valoriza a silhueta, proporcionando liberdade de movimento sem abrir mão do estilo.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Sem avaliação</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>['Conforto Superior', 'Barras Dobradas', 'Corte Casual', 'Detalhes de Acabamento', 'Fácil de Combinar']</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61mjwNm8C5L._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>1116x811</t>
+        </is>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Shorts e Bermudas</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_4?ie=UTF8&amp;node=17682127011</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Carregador Viagem USB-A Preto 15W Sem Cabo (Preto)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>R$39,99</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Carregador-Viagem-USB-Preto-Cabo/dp/B0DKPHB587/ref=sr_1_8?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-8&amp;xpid=tqkuqdh5H_SQg</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>Carregue seus dispositivos com rapidez e segurança onde quer que esteja com o Carregador Viagem USB-A Preto 15W. Ideal para quem está sempre em movimento, este carregador oferece potência e eficiência em um design compacto e fácil de transportar. Potência de 15W: Com uma saída de 15 watts, este carregador garante um carregamento rápido e eficiente para smartphones, tablets, fones de ouvido, e outros dispositivos USB-A, permitindo que você recupere energia de forma ágil, sem perder tempo. Design compacto e leve: Projetado para ser discreto e fácil de levar em bolsas, mochilas ou malas de viagem, ele é perfeito para acompanhar o seu ritmo, seja em viagens a trabalho ou lazer. USB-A universal: A porta USB-A oferece compatibilidade com uma ampla gama de cabos e dispositivos, garantindo flexibilidade para carregar praticamente qualquer gadget, desde que você tenha o cabo adequado. Sem cabo incluído: Este modelo não vem com cabo, oferecendo a liberdade de utilizar o cabo de sua escolha, seja para Android, iPhone ou outros dispositivos com diferentes entradas. Proteção integrada: Equipado com recursos de proteção contra superaquecimento, sobrecarga e curtos-circuitos, este carregador garante segurança durante o uso, protegendo seus dispositivos e você. Compatível com tensão global: Ideal para viajantes, o carregador pode ser utilizado em diferentes partes do mundo, adaptando-se a tensões de 100-240V, basta ter o adaptador de tomada correto. Dimensões: Compacto, fácil de guardar e transportar, pesando aproximadamente 50g. Leve com você o Carregador Viagem USB-A Preto 15W e garanta energia confiável para seus dispositivos em qualquer lugar Garantia do vendedor: 90 dias</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Sem avaliação</t>
         </is>
       </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>['Bullet points não encontrados']</t>
-        </is>
+      <c r="F9" t="n">
+        <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/51WYmEtPS1L._AC_SL1200_.jpg</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>2</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>833x1137</t>
+          <t>['Eficiência de Carregamento: Com potência de 15W, o carregador oferece carregamento rápido e eficiente para uma variedade de dispositivos, incluindo smartphones e tablets.', 'Portabilidade e Design Compacto: O design leve e discreto facilita o transporte em bolsas e mochilas, tornando-o ideal para quem está sempre em movimento.', 'Compatibilidade Universal: A porta USB-A permite a conexão com uma ampla gama de dispositivos, garantindo flexibilidade no carregamento.', 'Segurança Avançada: Equipado com proteção contra superaquecimento, sobrecarga e curtos-circuitos, assegura um uso seguro para os dispositivos.', 'Compatibilidade Global: Funciona em tensões de 100-240V, sendo ideal para viajantes que necessitam de um carregador confiável em diferentes regiões do mundo.']</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/41ybhWt-6iL._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>595x1185</t>
+        </is>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Carregadores de Parede</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16244307011</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Capa Protetora Kicktok para Galaxy S8 Plus, Samsung, Capa Protetora para Celular, Transparente</t>
+          <t>Ring Light 6 Polegadas 14cm com Mini Tripe (Preto)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R$31,23</t>
+          <t>R$30,90</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>A capa S8 kicktok protege o Galaxy S8 plus realçando o design do smartphone. A capa serve também como apoio permitindo uma posição confortável para visualização da tela ou para digitação além de permitir acesso rápido e fácil a todos os botões e conexões.</t>
+          <t>https://www.amazon.com.br/Ring-Light-Polegadas-Tripe-Preto/dp/B0DKPV57Z8/ref=sr_1_9?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-9&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3,8 de 5</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>7</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>['Estilo e elegância', 'Proteção completa contra riscos e quedas', 'Suporte embutido para assistir a vídeos com as mãos livres', 'País de Origem: VN']</t>
-        </is>
+          <t>Ring Light 6 Polegadas (14cm) com Mini Tripé! Ideal para criadores de conteúdo, maquiadores, youtubers e influenciadores, essa iluminação prática e eficiente é o segredo para resultados profissionais. Com seu design compacto e 3 opções de temperatura de cor (branca, neutra e quente), você terá o controle perfeito da luz, ajustando-a conforme o ambiente e o estilo de gravação. O mini tripé garante estabilidade e facilidade de uso em qualquer superfície, oferecendo ângulos ideais para selfies, gravações e videochamadas. Compacto, portátil e extremamente versátil, o Ring Light de 14cm é a escolha perfeita para destacar seus melhores momentos, melhorar a qualidade visual do seu conteúdo e proporcionar aquele brilho único que faz toda a diferença. Destaques: 3 modos de iluminação para ajuste perfeito; Mini tripé estável para qualquer superfície; Ideal para vídeos, fotos, lives e tutoriais; Compacto e leve, fácil de transportar.</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Sem avaliação</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/51jZ4MDpKBL._AC_SL1499_.jpg</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>4</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>681x1443</t>
+          <t>['Versatilidade de Iluminação: Com três opções de temperatura de cor (branca, neutra e quente), o Ring Light permite que você ajuste a iluminação conforme o ambiente e o estilo de gravação, garantindo resultados sempre profissionais.', 'Portabilidade e Design Compacto: Seu tamanho reduzido e leveza tornam este ring light extremamente fácil de transportar, ideal para criadores de conteúdo em movimento, maquiadores e influenciadores que precisam de uma solução prática.', 'Mini Tripé Estável: O mini tripé proporciona estabilidade em qualquer superfície, permitindo ângulos ideais para selfies, gravações e videochamadas, sem comprometer a qualidade da imagem.', 'Ideal para Múltiplas Aplicações: Perfeito para vídeos, fotos, transmissões ao vivo e tutoriais, o Ring Light é uma ferramenta essencial para quem deseja elevar a qualidade visual do seu conteúdo.', 'Facilidade de Uso: A combinação de um design intuitivo com a funcionalidade do tripé torna este ring light fácil de usar, proporcionando uma experiência sem complicações para todos os criadores de conteúdo, independentemente do nível de experiência.']</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/516F0uDJazL._AC_SL1200_.jpg</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>1200x1133</t>
+        </is>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Luzes de Selfie</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Luzes-Selfie-Telefone-Celular/b/ref=dp_bc_6?ie=UTF8&amp;node=23658796011</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Shorts Jeans Stillage Confortável com Barras Dobradas Estilo Casual</t>
+          <t>Capa Protetora Kicktok para Galaxy S8 Plus, Samsung, Capa Protetora para Celular, Transparente</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R$47,90</t>
+          <t>R$31,23</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Descubra o shorts perfeito para os dias quentes com o Shorts Jeans Stillage. Feito em jeans de alta qualidade, este modelo oferece o equilíbrio ideal entre conforto e estilo. Com barras dobradas que trazem um toque moderno e despojado, ele é a escolha ideal para compor looks casuais e frescos. Versátil, combina facilmente com blusas, camisetas ou regatas, sendo perfeito para passeios ou momentos descontraídos. Além disso, o corte ajustado valoriza a silhueta, proporcionando liberdade de movimento sem abrir mão do estilo.</t>
+          <t>https://www.amazon.com.br/Protetora-Kicktok-Samsung-Celular-Transparente/dp/B0777RX2H3/ref=sr_1_10?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-10&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Sem avaliação</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>['Bullet points não encontrados']</t>
-        </is>
+          <t>A capa S8 kicktok protege o Galaxy S8 plus realçando o design do smartphone. A capa serve também como apoio permitindo uma posição confortável para visualização da tela ou para digitação além de permitir acesso rápido e fácil a todos os botões e conexões.</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>3,8 de 5</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>7</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/61mjwNm8C5L._AC_SL1200_.jpg</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>2</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>1116x811</t>
+          <t>['Estilo e elegância', 'Proteção completa contra riscos e quedas', 'Suporte embutido para assistir a vídeos com as mãos livres', 'País de Origem: VN']</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51jZ4MDpKBL._AC_SL1499_.jpg</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>4</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Capas Laterais</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16244311011</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Película Protetora de Vidro Moto E5, Motorola, Transparente</t>
+          <t>Película Protetora de Vidro para Tela de Celular, para Motorola E4, Transparente</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R$14,44</t>
+          <t>R$19,09</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Proteção além da sua expectativa! As películas são compostas de um vidro temperado especial, não atrapalha o touch do seu smartphone, mas protege muito mais contra riscos, arranhões e impactos de menor grau sobre a tela do aparelho.</t>
+          <t>https://www.amazon.com.br/Pel%C3%ADcula-Protetora-Motorola-Celular-Transparente/dp/B075DZL4X6/ref=sr_1_11?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-11&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3,4 de 5</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>20</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>['Adesivo de silicone', 'Fina e forte', 'Alta sensibilidade', 'A tela do seu aparelho sempre nova']</t>
-        </is>
+          <t>Proteção além da sua expectativa. As películas são compostas de um vidro temperado especial, não atrapalha o touch do seu smartphone, mas protege muito mais contra riscos, arranhões e impactos de menor grau sobre a tela do aparelho.</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>4,3 de 5</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>31</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/71UPRh4y2oL._AC_SL1500_.jpg</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>2</v>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>724x1500</t>
+          <t>['Proteção além da sua expectativa', 'As películas são compostas de um vidro temperado especial, não atrapalha o touch do seu smartphone', 'Protege muito mais contra riscos, arranhões e impactos de menor grau sobre a tela do aparelho', 'Para Motorola E4']</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61HJECjobtL._AC_SL1000_.jpg</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>790x812</t>
+        </is>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Capas Laterais</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16244311011</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Capa Protetora Cristal Bumper Transparente com Lateral Moto G7, Motorola, 4882.0, Preta</t>
+          <t>Película Protetora de Vidro Moto E5, Motorola, Transparente</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R$45,41</t>
+          <t>R$14,44</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Protege seu smartphone na parte traseira e laterais, com abertura para acessórios como carregadores e fones. Para o uso de outros acessórios não precisa retirar a capa. Evite riscos e impactos que podem danificar seu aparelho. Com acabamento refinado, dá maior aderência e segurança quando o aparelho está em suas mãos.</t>
+          <t>https://www.amazon.com.br/Pel%C3%ADcula-Protetora-Transparente-Motorola-Celular/dp/B07F6LKG2V/ref=sr_1_12?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-12&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5 de 5</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>3</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>['Para o uso de outros acessórios não precisa retirar a capa', 'Evite riscos e impactos que podem danificar seu aparelho.', 'Com acabamento refinado, dá maior aderência e segurança quando o aparelho está em suas mãos.', 'País de Origem: CN']</t>
-        </is>
+          <t>Proteção além da sua expectativa! As películas são compostas de um vidro temperado especial, não atrapalha o touch do seu smartphone, mas protege muito mais contra riscos, arranhões e impactos de menor grau sobre a tela do aparelho.</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>3,4 de 5</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>20</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/615aJ73lEBL._AC_SL1500_.jpg</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
+          <t>['Adesivo de silicone', 'Fina e forte', 'Alta sensibilidade', 'A tela do seu aparelho sempre nova']</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/71UPRh4y2oL._AC_SL1500_.jpg</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
         <v>2</v>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>638x1500</t>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>724x1500</t>
+        </is>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Protetores de Tela</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Peliculas-Protetoras/b/ref=dp_bc_5?ie=UTF8&amp;node=16244091011</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Carregador Veicular Hightech, Energizer, EZ-DCA2CUWH3I, Branca</t>
+          <t>Capa Protetora Cristal Bumper Transparente com Lateral Moto G7, Motorola, 4882.0, Preta</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R$19,90</t>
+          <t>R$45,40</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Carregue seus aparelhos enquanto está na rua ou na estrada. Com 3, 4 Amp potência de saída, este carregador Veicular Energizer com duas saídas USB, proporciona a carga rápida e segura de seus smartphones ou tablets.</t>
+          <t>https://www.amazon.com.br/Protetora-Cristal-Transparente-Motorola-4882-0/dp/B07NDB5ZD9/ref=sr_1_13?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-13&amp;ufe=app_do%3Aamzn1.fos.6d798eae-cadf-45de-946a-f477d47705b9&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>4,5 de 5</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>11</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>['Carregue dois aparelhos simultaneamente', 'Obs: Não acompanha cabo USB', 'Design elegante']</t>
-        </is>
+          <t>Protege seu smartphone na parte traseira e laterais, com abertura para acessórios como carregadores e fones. Para o uso de outros acessórios não precisa retirar a capa. Evite riscos e impactos que podem danificar seu aparelho. Com acabamento refinado, dá maior aderência e segurança quando o aparelho está em suas mãos.</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>5 de 5</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>3</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/61t5kdNN+3L._AC_SL1500_.jpg</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
+          <t>['Para o uso de outros acessórios não precisa retirar a capa', 'Evite riscos e impactos que podem danificar seu aparelho.', 'Com acabamento refinado, dá maior aderência e segurança quando o aparelho está em suas mãos.', 'País de Origem: CN']</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/615aJ73lEBL._AC_SL1500_.jpg</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
         <v>2</v>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>1160x1248</t>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>638x1500</t>
+        </is>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Capas Laterais</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16244311011</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Capa Protetora Cristal Case Transparente Moto E5, Motorola, Capa com Proteção Completa (Carcaça+Tela), Transparente</t>
+          <t>Carregador Veicular Hightech, Energizer, EZ-DCA2CUWH3I, Branca</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R$14,90</t>
+          <t>R$19,90</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Protege seu smartphone na parte traseira e laterais. com abertura para acessórios como carregadores e fones. Para o uso de outros acessórios não precisa retirar a capa. Evite riscos e impactos que podem danificar seu aparelho.</t>
+          <t>https://www.amazon.com.br/Carregador-Veicular-Original-Energizer-Sa%C3%ADdas/dp/B0182JTL9G/ref=sr_1_14?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-14&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3,2 de 5</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>33</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>['Protege seu smartphone na parte traseira e laterais. com abertura para acessórios como carregadores e fones', 'Para o uso de outros acessórios não precisa retirar a capa', 'Evite riscos e impactos que podem danificar seu aparelho', 'País de Origem: CN']</t>
-        </is>
+          <t>Carregue seus aparelhos enquanto está na rua ou na estrada. Com 3, 4 Amp potência de saída, este carregador Veicular Energizer com duas saídas USB, proporciona a carga rápida e segura de seus smartphones ou tablets.</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>4,5 de 5</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>12</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/611KhH7BtTL._AC_SL1500_.jpg</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>697x1433</t>
+          <t>['Carregue dois aparelhos simultaneamente', 'Obs: Não acompanha cabo USB', 'Design elegante']</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61t5kdNN+3L._AC_SL1500_.jpg</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>2</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>1160x1248</t>
+        </is>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Carregadores Veiculares</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Carregadores-Veiculares/b/ref=dp_bc_5?ie=UTF8&amp;node=16244303011</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Cabo Displayport 4k Blindado Macho X Macho 1,8m 1.1 E 1.2 (preto)</t>
+          <t>Capa Protetora Cristal Case Transparente Moto E5, Motorola, Capa com Proteção Completa (Carcaça+Tela), Transparente</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>R$31,90</t>
+          <t>R$14,90</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>O Cabo DisplayPort 4K Blindado de 1,8 metros oferece qualidade de transmissão superior para quem busca desempenho e durabilidade. Com conectores banhados a ouro e blindagem reforçada, ele proporciona máxima proteção contra interferências e uma conexão estável. Ideal para quem exige alta definição em resoluções de até 4K, este cabo é perfeito para conectar notebooks, tablets, TVs, monitores e projetores com suporte DisplayPort. Características do Produto: Marca: F3 Modelo: JC-DP1.8 Resolução Suportada: 480i, 576i/p, 720i/p, 1080i/p, até 2160p (4K) Conectores: 2 x DisplayPort (Macho) com conectores banhados a ouro Padrões Compatíveis: DisplayPort 1.1 e 1.2 Comprimento do Cabo: 1,8 metro Cor: Preto Com trava de segurança, garantindo uma conexão firme e confiável. Garantia do vendedor: 90 dias</t>
+          <t>https://www.amazon.com.br/Protetora-Transparente-Motorola-Prote%C3%A7%C3%A3o-Completa/dp/B07F7JXDVY/ref=sr_1_15?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-15&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Sem avaliação</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>['Alta Resolução: Suporta resoluções de até 4K (2160p), proporcionando imagens nítidas e detalhadas, ideal para gamers e profissionais que exigem qualidade visual superior.', 'Blindagem Reforçada: A blindagem avançada do cabo protege contra interferências eletromagnéticas, minimizando perda de sinal e garantindo uma conexão de alta qualidade.', 'Conectores Banhados a Ouro: Os conectores banhados a ouro garantem uma excelente condutividade e resistência à corrosão, assegurando uma transmissão de sinal mais estável e confiável.', 'Trava de Segurança: Equipado com uma trava de segurança, o cabo assegura uma conexão firme e confiável, evitando desconexões acidentais durante o uso.', 'Comprimento Ideal: Com 1,8 metros de comprimento, o cabo oferece flexibilidade e conveniência para conectar dispositivos em diferentes configurações sem comprometer a qualidade do sinal.']</t>
-        </is>
+          <t>Protege seu smartphone na parte traseira e laterais. com abertura para acessórios como carregadores e fones. Para o uso de outros acessórios não precisa retirar a capa. Evite riscos e impactos que podem danificar seu aparelho.</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>3,2 de 5</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>33</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/51-3+Xs2w-L._AC_SL1200_.jpg</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
+          <t>['Protege seu smartphone na parte traseira e laterais. com abertura para acessórios como carregadores e fones', 'Para o uso de outros acessórios não precisa retirar a capa', 'Evite riscos e impactos que podem danificar seu aparelho', 'País de Origem: CN']</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/611KhH7BtTL._AC_SL1500_.jpg</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
         <v>1</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>1200x1091</t>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>697x1433</t>
+        </is>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Capas Laterais</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16244311011</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Carregador Viagem USB-A Preto 15W Sem Cabo (Preto)</t>
+          <t>Conj para Bar em Inox Stem 5 Pçs Prana Inox</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>R$39,99</t>
+          <t>R$199,90</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Carregue seus dispositivos com rapidez e segurança onde quer que esteja com o Carregador Viagem USB-A Preto 15W. Ideal para quem está sempre em movimento, este carregador oferece potência e eficiência em um design compacto e fácil de transportar. Potência de 15W: Com uma saída de 15 watts, este carregador garante um carregamento rápido e eficiente para smartphones, tablets, fones de ouvido, e outros dispositivos USB-A, permitindo que você recupere energia de forma ágil, sem perder tempo. Design compacto e leve: Projetado para ser discreto e fácil de levar em bolsas, mochilas ou malas de viagem, ele é perfeito para acompanhar o seu ritmo, seja em viagens a trabalho ou lazer. USB-A universal: A porta USB-A oferece compatibilidade com uma ampla gama de cabos e dispositivos, garantindo flexibilidade para carregar praticamente qualquer gadget, desde que você tenha o cabo adequado. Sem cabo incluído: Este modelo não vem com cabo, oferecendo a liberdade de utilizar o cabo de sua escolha, seja para Android, iPhone ou outros dispositivos com diferentes entradas. Proteção integrada: Equipado com recursos de proteção contra superaquecimento, sobrecarga e curtos-circuitos, este carregador garante segurança durante o uso, protegendo seus dispositivos e você. Compatível com tensão global: Ideal para viajantes, o carregador pode ser utilizado em diferentes partes do mundo, adaptando-se a tensões de 100-240V, basta ter o adaptador de tomada correto. Dimensões: Compacto, fácil de guardar e transportar, pesando aproximadamente 50g. Leve com você o Carregador Viagem USB-A Preto 15W e garanta energia confiável para seus dispositivos em qualquer lugar Garantia do vendedor: 90 dias</t>
+          <t>https://www.amazon.com.br/CONJ-PARA-PRANA-Prana-000BS04008XXXNMS/dp/B07C1PYNZY/ref=sr_1_16?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-16&amp;ufe=app_do%3Aamzn1.fos.6121c6c4-c969-43ae-92f7-cc248fc6181d&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>Conj. Bar stem em aço inox no modelo liso. Contém peneira, faca, dosador, pinça. Todo feito em inox polido, deixa o lugar sofisticado como decoração e muito útil no preparo de drinks e bebidas com tudo o que é preciso para um preparo rápido.</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>Sem avaliação</t>
         </is>
       </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>['Eficiência de Carregamento: Com potência de 15W, o carregador oferece carregamento rápido e eficiente para uma variedade de dispositivos, incluindo smartphones e tablets.', 'Portabilidade e Design Compacto: O design leve e discreto facilita o transporte em bolsas e mochilas, tornando-o ideal para quem está sempre em movimento.', 'Compatibilidade Universal: A porta USB-A permite a conexão com uma ampla gama de dispositivos, garantindo flexibilidade no carregamento.', 'Segurança Avançada: Equipado com proteção contra superaquecimento, sobrecarga e curtos-circuitos, assegura um uso seguro para os dispositivos.', 'Compatibilidade Global: Funciona em tensões de 100-240V, sendo ideal para viajantes que necessitam de um carregador confiável em diferentes regiões do mundo.']</t>
-        </is>
+      <c r="F17" t="n">
+        <v>0</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/41ybhWt-6iL._AC_SL1200_.jpg</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>1</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>595x1185</t>
+          <t>['Com Design Limpo E Moderno, Trazendo Requinte E Sofisticação Para A Decoração De Seu Bar', 'Um Lindo Presente Para Homens Modernos Que Gostam De Preparar Seus Dinks Ou Receber Seus Convidados Com Elegncia', 'Em Aço Inox Polido, Prática De Limpar E Durável', 'País de Origem: CN']</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/51n-vWG4HIL._AC_SL1000_.jpg</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>5</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>611x893</t>
+        </is>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Kits para Bar</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_4?ie=UTF8&amp;node=17125148011</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Conj para Bar em Inox Stem 5 Pçs Prana Inox</t>
+          <t>Moldura Dobravel Plastica Crismop Inox</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R$199,90</t>
+          <t>R$14,90</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Conj. Bar stem em aço inox no modelo liso. Contém peneira, faca, dosador, pinça. Todo feito em inox polido, deixa o lugar sofisticado como decoração e muito útil no preparo de drinks e bebidas com tudo o que é preciso para um preparo rápido.</t>
+          <t>https://www.amazon.com.br/Moldura-Dobravel-Plastica-Crismop-Inox/dp/B07GFW29QF/ref=sr_1_17?dib=eyJ2IjoiMSJ9.nJUGtznzO1_mp8QWZsUFXw.U2CihjVDI-ycq8hPBej8kXlvKnB5OP9svp036lzUguc&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748834&amp;s=merchant-items&amp;sr=1-17&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Sem avaliação</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>['Com Design Limpo E Moderno, Trazendo Requinte E Sofisticação Para A Decoração De Seu Bar', 'Um Lindo Presente Para Homens Modernos Que Gostam De Preparar Seus Dinks Ou Receber Seus Convidados Com Elegncia', 'Em Aço Inox Polido, Prática De Limpar E Durável', 'País de Origem: CN']</t>
-        </is>
+          <t>Suporte para Mop Pó Dobrável, prático e leve, ideal para ser usado com o refil mop algodão ou microfibra com 45cm, sua casa sem pó. Muito mais praticidade e rapidez na limpeza de sua casa ou apartamento.</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>5 de 5</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>2</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/51n-vWG4HIL._AC_SL1000_.jpg</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>5</v>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>611x893</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Moldura Dobravel Plastica Crismop Inox</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>R$14,90</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Suporte para Mop Pó Dobrável, prático e leve, ideal para ser usado com o refil mop algodão ou microfibra com 45cm, sua casa sem pó. Muito mais praticidade e rapidez na limpeza de sua casa ou apartamento.</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>5 de 5</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>2</v>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
           <t>['Ideal para limpar e tirar o pó na sala no quarto ou no seu escritório', 'Dobrável em aço e plástico com 45 cm', 'Material pp e aço inox', 'Fabricado com muito cuidado e atenção aos detalhes']</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>https://m.media-amazon.com/images/I/41n99saqHAL._AC_SL1000_.jpg</t>
         </is>
       </c>
-      <c r="H19" t="n">
+      <c r="I18" t="n">
         <v>1</v>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>410x362</t>
+        </is>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Porta-Retratos de Mesa e Parede</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=17100787011</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
+ Adicionada função de coletar a data da extração. + Adicionada função de coletar ranking de determinado produto. - Removida parte da função salvar_produtos_em_csv. (Foi removida a parte que a função salva o csv com um nome dinâmico - de acordo com a conta que está sendo analisada no momento - )
</commit_message>
<xml_diff>
--- a/arquivo_convertido.xlsx
+++ b/arquivo_convertido.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,7 +496,22 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>link_categoria</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>fba</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>data_coleta</t>
         </is>
       </c>
     </row>
@@ -513,7 +528,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Portas-Leitor-Cartao-Memoria-7portas/dp/B0DGGW72LL/ref=sr_1_1?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-1&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Portas-Leitor-Cartao-Memoria-7portas/dp/B0DGGW72LL/ref=sr_1_1?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-1&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -583,7 +598,22 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
+          <t>863</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
           <t>https://www.amazon.com.br/Hubs-USB/b/ref=dp_bc_3?ie=UTF8&amp;node=23884302011</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
@@ -600,7 +630,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Bermuda-Masculina-T%C3%A9rmica-Compress%C3%A3o-I-Max/dp/B0DGQTCMC5/ref=sr_1_2?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-2&amp;ufe=app_do%3Aamzn1.fos.a492fd4a-f54d-4e8d-8c31-35e0a04ce61e&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Bermuda-Masculina-T%C3%A9rmica-Compress%C3%A3o-I-Max/dp/B0DGQTCMC5/ref=sr_1_2?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-2&amp;ufe=app_do%3Aamzn1.fos.a492fd4a-f54d-4e8d-8c31-35e0a04ce61e&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -653,34 +683,44 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
+          <t>Indisponível</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
           <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=17682478011</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Biquíni Aviação Estampado Sem Bojo Conforto e Estilo</t>
+          <t>Capa Protetora Defender Preta Para Galaxy Tab III 7 Otterbox (Preto)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R$44,99</t>
+          <t>R$28,89</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Biqu%C3%ADni-Avia%C3%A7%C3%A3o-Estampado-Conforto-Estilo/dp/B0DKQY7HWC/ref=sr_1_3?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-3&amp;ufe=app_do%3Aamzn1.fos.6d798eae-cadf-45de-946a-f477d47705b9&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Protetora-Defender-Preta-Galaxy-Otterbox/dp/B07QYV9KGQ/ref=sr_1_3?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-3&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Transforme seu Verão com o Biquíni Aviação com Estampa Pimenta
-Prepare-se para brilhar neste verão com o Biquíni Aviação com Estampa Pimenta. Com um design vibrante e ousado, este biquíni é perfeito para quem deseja se destacar à beira da piscina ou na praia. A estampa de pimenta traz um toque de personalidade e modernidade, tornando cada momento ainda mais especial.
-Estampa Exclusiva: A estampa de pimenta não só adiciona um charme único e vibrante ao seu visual, mas também reflete seu estilo arrojado e confiante.
-Conforto Sem Bojo: A ausência de bojo garante um ajuste leve e confortável, ideal para dias ensolarados de diversão e relaxamento. Você pode se mover livremente, sem abrir mão da elegância.
-Design Estiloso: Com um corte que valoriza as curvas, este biquíni é ideal para quem busca um look ousado e contemporâneo. Combine-o com seus acessórios favoritos e esteja pronta para arrasar!
-Transforme suas experiências de verão em momentos inesquecíveis com o Biquíni Aviação. Sinta-se confiante, estilosa e confortável em qualquer ocasião!</t>
+          <t>Proteja seu Galaxy Tab III 7 com a Capa Protetora Defender da Otterbox, projetada para oferecer máxima segurança e funcionalidade. Esta capa é ideal para quem busca proteção robusta sem abrir mão do estilo. Características: - Proteção Superior: A tecnologia de absorção de impactos proporciona defesa contra quedas, arranhões e impactos, garantindo que seu dispositivo permaneça em perfeito estado. - Design Ergonômico: Com um encaixe seguro e confortável, a capa facilita o manuseio, permitindo que você utilize seu tablet com facilidade. - Acesso Total: A Capa Defender mantém todas as portas e botões acessíveis, permitindo o uso total das funcionalidades do seu Galaxy Tab III 7, sem a necessidade de remover a capa. - Material de Alta Qualidade: Fabricada com materiais duráveis, resistentes à abrasão e ao desgaste, garantindo longa vida útil. - Instalação Simples: A capa é fácil de instalar e remover, permitindo que você troque de acessório conforme suas necessidades. Dimensões e Peso: - Compatível com Galaxy Tab III 7. - Peso leve, ideal para transporte. Cores Disponíveis: - Preto clássico, que combina com qualquer estilo. Cuidados e Manutenção: - Limpeza com pano úmido. - Evitar contato com produtos químicos agressivos. Garanta a proteção que seu Galaxy Tab III 7 merece com a Capa Protetora Defender Preta da Otterbox. Perfeita para uso diário, viagens ou qualquer situação em que seu tablet esteja exposto a riscos.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -693,20 +733,20 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>['Detalhes da estampa de pimenta e seu charme único', 'Conforto durante atividades', 'Valoriza as curvas e complementa o visual', 'Design Vibrante e Ousado']</t>
+          <t>['Proteção em Camadas: A capa possui três camadas de proteção, incluindo uma camada interna de policarbonato rígido que absorve impactos e uma camada externa emborrachada que oferece resistência adicional contra quedas e arranhões.', 'Design Resistente: A capa é projetada para suportar ambientes desafiadores e testes rigorosos, protegendo o dispositivo de quedas de até 2 metros', 'Acesso Total: Apesar da proteção, a capa permite fácil acesso a todos os botões, portas e funcionalidades do tablet, incluindo câmera e conector de carregamento, sem precisar remover a capa.', 'Material e Dimensões: A capa é feita de policarbonato e silicone emborrachado, leve e projetada para se ajustar perfeitamente ao Galaxy Tab III 7".']</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/61jwBveWy3L._AC_SL1200_.jpg</t>
+          <t>https://m.media-amazon.com/images/I/41Vc49XdKZL._AC_SL1200_.jpg</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>797x1034</t>
+          <t>498x1148</t>
         </is>
       </c>
       <c r="K4" t="b">
@@ -714,12 +754,27 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Conjuntos</t>
+          <t>Capas, Bolsas e Estojos</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/b/ref=dp_bc_6?ie=UTF8&amp;node=17682696011</t>
+          <t>Indisponível</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_4?ie=UTF8&amp;node=16364864011</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
@@ -736,7 +791,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Cuecas-Boxer-Mash-Preto-Listrado/dp/B0DGXZJ3TZ/ref=sr_1_4?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-4&amp;ufe=app_do%3Aamzn1.fos.6d798eae-cadf-45de-946a-f477d47705b9&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Cuecas-Boxer-Mash-Preto-Listrado/dp/B0DGXZJ3TZ/ref=sr_1_4?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-4&amp;ufe=app_do%3Aamzn1.fos.6d798eae-cadf-45de-946a-f477d47705b9&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -793,29 +848,44 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
+          <t>Indisponível</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
           <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=17682497011</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Capa Protetora Defender Preta Para Galaxy Tab III 7 Otterbox (Preto)</t>
+          <t>Cabo Displayport 4k Blindado Macho X Macho 1,8m 1.1 E 1.2 (preto)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$28,89</t>
+          <t>R$31,90</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Protetora-Defender-Preta-Galaxy-Otterbox/dp/B07QYV9KGQ/ref=sr_1_5?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-5&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Cabo-Displayport-Blindado-Macho-preto/dp/B0DKPHT6SJ/ref=sr_1_5?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-5&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Proteja seu Galaxy Tab III 7 com a Capa Protetora Defender da Otterbox, projetada para oferecer máxima segurança e funcionalidade. Esta capa é ideal para quem busca proteção robusta sem abrir mão do estilo. Características: - Proteção Superior: A tecnologia de absorção de impactos proporciona defesa contra quedas, arranhões e impactos, garantindo que seu dispositivo permaneça em perfeito estado. - Design Ergonômico: Com um encaixe seguro e confortável, a capa facilita o manuseio, permitindo que você utilize seu tablet com facilidade. - Acesso Total: A Capa Defender mantém todas as portas e botões acessíveis, permitindo o uso total das funcionalidades do seu Galaxy Tab III 7, sem a necessidade de remover a capa. - Material de Alta Qualidade: Fabricada com materiais duráveis, resistentes à abrasão e ao desgaste, garantindo longa vida útil. - Instalação Simples: A capa é fácil de instalar e remover, permitindo que você troque de acessório conforme suas necessidades. Dimensões e Peso: - Compatível com Galaxy Tab III 7. - Peso leve, ideal para transporte. Cores Disponíveis: - Preto clássico, que combina com qualquer estilo. Cuidados e Manutenção: - Limpeza com pano úmido. - Evitar contato com produtos químicos agressivos. Garanta a proteção que seu Galaxy Tab III 7 merece com a Capa Protetora Defender Preta da Otterbox. Perfeita para uso diário, viagens ou qualquer situação em que seu tablet esteja exposto a riscos.</t>
+          <t>O Cabo DisplayPort 4K Blindado de 1,8 metros oferece qualidade de transmissão superior para quem busca desempenho e durabilidade. Com conectores banhados a ouro e blindagem reforçada, ele proporciona máxima proteção contra interferências e uma conexão estável. Ideal para quem exige alta definição em resoluções de até 4K, este cabo é perfeito para conectar notebooks, tablets, TVs, monitores e projetores com suporte DisplayPort. Características do Produto: Marca: F3 Modelo: JC-DP1.8 Resolução Suportada: 480i, 576i/p, 720i/p, 1080i/p, até 2160p (4K) Conectores: 2 x DisplayPort (Macho) com conectores banhados a ouro Padrões Compatíveis: DisplayPort 1.1 e 1.2 Comprimento do Cabo: 1,8 metro Cor: Preto Com trava de segurança, garantindo uma conexão firme e confiável. Garantia do vendedor: 90 dias</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -828,20 +898,20 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['Proteção em Camadas: A capa possui três camadas de proteção, incluindo uma camada interna de policarbonato rígido que absorve impactos e uma camada externa emborrachada que oferece resistência adicional contra quedas e arranhões.', 'Design Resistente: A capa é projetada para suportar ambientes desafiadores e testes rigorosos, protegendo o dispositivo de quedas de até 2 metros', 'Acesso Total: Apesar da proteção, a capa permite fácil acesso a todos os botões, portas e funcionalidades do tablet, incluindo câmera e conector de carregamento, sem precisar remover a capa.', 'Material e Dimensões: A capa é feita de policarbonato e silicone emborrachado, leve e projetada para se ajustar perfeitamente ao Galaxy Tab III 7".']</t>
+          <t>['Alta Resolução: Suporta resoluções de até 4K (2160p), proporcionando imagens nítidas e detalhadas, ideal para gamers e profissionais que exigem qualidade visual superior.', 'Blindagem Reforçada: A blindagem avançada do cabo protege contra interferências eletromagnéticas, minimizando perda de sinal e garantindo uma conexão de alta qualidade.', 'Conectores Banhados a Ouro: Os conectores banhados a ouro garantem uma excelente condutividade e resistência à corrosão, assegurando uma transmissão de sinal mais estável e confiável.', 'Trava de Segurança: Equipado com uma trava de segurança, o cabo assegura uma conexão firme e confiável, evitando desconexões acidentais durante o uso.', 'Comprimento Ideal: Com 1,8 metros de comprimento, o cabo oferece flexibilidade e conveniência para conectar dispositivos em diferentes configurações sem comprometer a qualidade do sinal.']</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/41Vc49XdKZL._AC_SL1200_.jpg</t>
+          <t>https://m.media-amazon.com/images/I/51-3+Xs2w-L._AC_SL1200_.jpg</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>498x1148</t>
+          <t>1200x1091</t>
         </is>
       </c>
       <c r="K6" t="b">
@@ -849,34 +919,54 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Capas, Bolsas e Estojos</t>
+          <t>Cabos DisplayPort</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/b/ref=dp_bc_4?ie=UTF8&amp;node=16364864011</t>
+          <t>Indisponível</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16364884011</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cabo Displayport 4k Blindado Macho X Macho 1,8m 1.1 E 1.2 (preto)</t>
+          <t>Biquíni Aviação Estampado Sem Bojo Conforto e Estilo</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$31,90</t>
+          <t>R$44,99</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Cabo-Displayport-Blindado-Macho-preto/dp/B0DKPHT6SJ/ref=sr_1_6?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-6&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Biqu%C3%ADni-Avia%C3%A7%C3%A3o-Estampado-Conforto-Estilo/dp/B0DKQY7HWC/ref=sr_1_6?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-6&amp;ufe=app_do%3Aamzn1.fos.6d798eae-cadf-45de-946a-f477d47705b9&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>O Cabo DisplayPort 4K Blindado de 1,8 metros oferece qualidade de transmissão superior para quem busca desempenho e durabilidade. Com conectores banhados a ouro e blindagem reforçada, ele proporciona máxima proteção contra interferências e uma conexão estável. Ideal para quem exige alta definição em resoluções de até 4K, este cabo é perfeito para conectar notebooks, tablets, TVs, monitores e projetores com suporte DisplayPort. Características do Produto: Marca: F3 Modelo: JC-DP1.8 Resolução Suportada: 480i, 576i/p, 720i/p, 1080i/p, até 2160p (4K) Conectores: 2 x DisplayPort (Macho) com conectores banhados a ouro Padrões Compatíveis: DisplayPort 1.1 e 1.2 Comprimento do Cabo: 1,8 metro Cor: Preto Com trava de segurança, garantindo uma conexão firme e confiável. Garantia do vendedor: 90 dias</t>
+          <t>Transforme seu Verão com o Biquíni Aviação com Estampa Pimenta
+Prepare-se para brilhar neste verão com o Biquíni Aviação com Estampa Pimenta. Com um design vibrante e ousado, este biquíni é perfeito para quem deseja se destacar à beira da piscina ou na praia. A estampa de pimenta traz um toque de personalidade e modernidade, tornando cada momento ainda mais especial.
+Estampa Exclusiva: A estampa de pimenta não só adiciona um charme único e vibrante ao seu visual, mas também reflete seu estilo arrojado e confiante.
+Conforto Sem Bojo: A ausência de bojo garante um ajuste leve e confortável, ideal para dias ensolarados de diversão e relaxamento. Você pode se mover livremente, sem abrir mão da elegância.
+Design Estiloso: Com um corte que valoriza as curvas, este biquíni é ideal para quem busca um look ousado e contemporâneo. Combine-o com seus acessórios favoritos e esteja pronta para arrasar!
+Transforme suas experiências de verão em momentos inesquecíveis com o Biquíni Aviação. Sinta-se confiante, estilosa e confortável em qualquer ocasião!</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -889,20 +979,20 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['Alta Resolução: Suporta resoluções de até 4K (2160p), proporcionando imagens nítidas e detalhadas, ideal para gamers e profissionais que exigem qualidade visual superior.', 'Blindagem Reforçada: A blindagem avançada do cabo protege contra interferências eletromagnéticas, minimizando perda de sinal e garantindo uma conexão de alta qualidade.', 'Conectores Banhados a Ouro: Os conectores banhados a ouro garantem uma excelente condutividade e resistência à corrosão, assegurando uma transmissão de sinal mais estável e confiável.', 'Trava de Segurança: Equipado com uma trava de segurança, o cabo assegura uma conexão firme e confiável, evitando desconexões acidentais durante o uso.', 'Comprimento Ideal: Com 1,8 metros de comprimento, o cabo oferece flexibilidade e conveniência para conectar dispositivos em diferentes configurações sem comprometer a qualidade do sinal.']</t>
+          <t>['Detalhes da estampa de pimenta e seu charme único', 'Conforto durante atividades', 'Valoriza as curvas e complementa o visual', 'Design Vibrante e Ousado']</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/51-3+Xs2w-L._AC_SL1200_.jpg</t>
+          <t>https://m.media-amazon.com/images/I/61jwBveWy3L._AC_SL1200_.jpg</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>1200x1091</t>
+          <t>797x1034</t>
         </is>
       </c>
       <c r="K7" t="b">
@@ -910,34 +1000,49 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Cabos DisplayPort</t>
+          <t>Conjuntos</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16364884011</t>
+          <t>Indisponível</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_6?ie=UTF8&amp;node=17682696011</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Shorts Jeans Stillage Confortável com Barras Dobradas Estilo Casual</t>
+          <t>Carregador Viagem USB-A Preto 15W Sem Cabo (Preto)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$47,90</t>
+          <t>R$39,99</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Shorts-Stillage-Confort%C3%A1vel-Barras-Dobradas/dp/B0DGXZDBPY/ref=sr_1_7?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-7&amp;ufe=app_do%3Aamzn1.fos.6d798eae-cadf-45de-946a-f477d47705b9&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Carregador-Viagem-USB-Preto-Cabo/dp/B0DKPHB587/ref=sr_1_7?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-7&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Descubra o shorts perfeito para os dias quentes com o Shorts Jeans Stillage. Feito em jeans de alta qualidade, este modelo oferece o equilíbrio ideal entre conforto e estilo. Com barras dobradas que trazem um toque moderno e despojado, ele é a escolha ideal para compor looks casuais e frescos. Versátil, combina facilmente com blusas, camisetas ou regatas, sendo perfeito para passeios ou momentos descontraídos. Além disso, o corte ajustado valoriza a silhueta, proporcionando liberdade de movimento sem abrir mão do estilo.</t>
+          <t>Carregue seus dispositivos com rapidez e segurança onde quer que esteja com o Carregador Viagem USB-A Preto 15W. Ideal para quem está sempre em movimento, este carregador oferece potência e eficiência em um design compacto e fácil de transportar. Potência de 15W: Com uma saída de 15 watts, este carregador garante um carregamento rápido e eficiente para smartphones, tablets, fones de ouvido, e outros dispositivos USB-A, permitindo que você recupere energia de forma ágil, sem perder tempo. Design compacto e leve: Projetado para ser discreto e fácil de levar em bolsas, mochilas ou malas de viagem, ele é perfeito para acompanhar o seu ritmo, seja em viagens a trabalho ou lazer. USB-A universal: A porta USB-A oferece compatibilidade com uma ampla gama de cabos e dispositivos, garantindo flexibilidade para carregar praticamente qualquer gadget, desde que você tenha o cabo adequado. Sem cabo incluído: Este modelo não vem com cabo, oferecendo a liberdade de utilizar o cabo de sua escolha, seja para Android, iPhone ou outros dispositivos com diferentes entradas. Proteção integrada: Equipado com recursos de proteção contra superaquecimento, sobrecarga e curtos-circuitos, este carregador garante segurança durante o uso, protegendo seus dispositivos e você. Compatível com tensão global: Ideal para viajantes, o carregador pode ser utilizado em diferentes partes do mundo, adaptando-se a tensões de 100-240V, basta ter o adaptador de tomada correto. Dimensões: Compacto, fácil de guardar e transportar, pesando aproximadamente 50g. Leve com você o Carregador Viagem USB-A Preto 15W e garanta energia confiável para seus dispositivos em qualquer lugar Garantia do vendedor: 90 dias</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -950,20 +1055,20 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['Conforto Superior', 'Barras Dobradas', 'Corte Casual', 'Detalhes de Acabamento', 'Fácil de Combinar']</t>
+          <t>['Eficiência de Carregamento: Com potência de 15W, o carregador oferece carregamento rápido e eficiente para uma variedade de dispositivos, incluindo smartphones e tablets.', 'Portabilidade e Design Compacto: O design leve e discreto facilita o transporte em bolsas e mochilas, tornando-o ideal para quem está sempre em movimento.', 'Compatibilidade Universal: A porta USB-A permite a conexão com uma ampla gama de dispositivos, garantindo flexibilidade no carregamento.', 'Segurança Avançada: Equipado com proteção contra superaquecimento, sobrecarga e curtos-circuitos, assegura um uso seguro para os dispositivos.', 'Compatibilidade Global: Funciona em tensões de 100-240V, sendo ideal para viajantes que necessitam de um carregador confiável em diferentes regiões do mundo.']</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/61mjwNm8C5L._AC_SL1200_.jpg</t>
+          <t>https://m.media-amazon.com/images/I/41ybhWt-6iL._AC_SL1200_.jpg</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>1116x811</t>
+          <t>595x1185</t>
         </is>
       </c>
       <c r="K8" t="b">
@@ -971,34 +1076,49 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Shorts e Bermudas</t>
+          <t>Carregadores de Parede</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/b/ref=dp_bc_4?ie=UTF8&amp;node=17682127011</t>
+          <t>Indisponível</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16244307011</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Carregador Viagem USB-A Preto 15W Sem Cabo (Preto)</t>
+          <t>Shorts Jeans Stillage Confortável com Barras Dobradas Estilo Casual</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$39,99</t>
+          <t>R$47,90</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Carregador-Viagem-USB-Preto-Cabo/dp/B0DKPHB587/ref=sr_1_8?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-8&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Shorts-Stillage-Confort%C3%A1vel-Barras-Dobradas/dp/B0DGXZDBPY/ref=sr_1_8?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-8&amp;ufe=app_do%3Aamzn1.fos.6d798eae-cadf-45de-946a-f477d47705b9&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Carregue seus dispositivos com rapidez e segurança onde quer que esteja com o Carregador Viagem USB-A Preto 15W. Ideal para quem está sempre em movimento, este carregador oferece potência e eficiência em um design compacto e fácil de transportar. Potência de 15W: Com uma saída de 15 watts, este carregador garante um carregamento rápido e eficiente para smartphones, tablets, fones de ouvido, e outros dispositivos USB-A, permitindo que você recupere energia de forma ágil, sem perder tempo. Design compacto e leve: Projetado para ser discreto e fácil de levar em bolsas, mochilas ou malas de viagem, ele é perfeito para acompanhar o seu ritmo, seja em viagens a trabalho ou lazer. USB-A universal: A porta USB-A oferece compatibilidade com uma ampla gama de cabos e dispositivos, garantindo flexibilidade para carregar praticamente qualquer gadget, desde que você tenha o cabo adequado. Sem cabo incluído: Este modelo não vem com cabo, oferecendo a liberdade de utilizar o cabo de sua escolha, seja para Android, iPhone ou outros dispositivos com diferentes entradas. Proteção integrada: Equipado com recursos de proteção contra superaquecimento, sobrecarga e curtos-circuitos, este carregador garante segurança durante o uso, protegendo seus dispositivos e você. Compatível com tensão global: Ideal para viajantes, o carregador pode ser utilizado em diferentes partes do mundo, adaptando-se a tensões de 100-240V, basta ter o adaptador de tomada correto. Dimensões: Compacto, fácil de guardar e transportar, pesando aproximadamente 50g. Leve com você o Carregador Viagem USB-A Preto 15W e garanta energia confiável para seus dispositivos em qualquer lugar Garantia do vendedor: 90 dias</t>
+          <t>Descubra o shorts perfeito para os dias quentes com o Shorts Jeans Stillage. Feito em jeans de alta qualidade, este modelo oferece o equilíbrio ideal entre conforto e estilo. Com barras dobradas que trazem um toque moderno e despojado, ele é a escolha ideal para compor looks casuais e frescos. Versátil, combina facilmente com blusas, camisetas ou regatas, sendo perfeito para passeios ou momentos descontraídos. Além disso, o corte ajustado valoriza a silhueta, proporcionando liberdade de movimento sem abrir mão do estilo.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1011,20 +1131,20 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['Eficiência de Carregamento: Com potência de 15W, o carregador oferece carregamento rápido e eficiente para uma variedade de dispositivos, incluindo smartphones e tablets.', 'Portabilidade e Design Compacto: O design leve e discreto facilita o transporte em bolsas e mochilas, tornando-o ideal para quem está sempre em movimento.', 'Compatibilidade Universal: A porta USB-A permite a conexão com uma ampla gama de dispositivos, garantindo flexibilidade no carregamento.', 'Segurança Avançada: Equipado com proteção contra superaquecimento, sobrecarga e curtos-circuitos, assegura um uso seguro para os dispositivos.', 'Compatibilidade Global: Funciona em tensões de 100-240V, sendo ideal para viajantes que necessitam de um carregador confiável em diferentes regiões do mundo.']</t>
+          <t>['Conforto Superior', 'Barras Dobradas', 'Corte Casual', 'Detalhes de Acabamento', 'Fácil de Combinar']</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/41ybhWt-6iL._AC_SL1200_.jpg</t>
+          <t>https://m.media-amazon.com/images/I/61mjwNm8C5L._AC_SL1200_.jpg</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>595x1185</t>
+          <t>1116x811</t>
         </is>
       </c>
       <c r="K9" t="b">
@@ -1032,12 +1152,27 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Carregadores de Parede</t>
+          <t>Shorts e Bermudas</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16244307011</t>
+          <t>Indisponível</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_4?ie=UTF8&amp;node=17682127011</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
@@ -1054,7 +1189,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Ring-Light-Polegadas-Tripe-Preto/dp/B0DKPV57Z8/ref=sr_1_9?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-9&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Ring-Light-Polegadas-Tripe-Preto/dp/B0DKPV57Z8/ref=sr_1_9?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-9&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1098,7 +1233,22 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
+          <t>Indisponível</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
           <t>https://www.amazon.com.br/Luzes-Selfie-Telefone-Celular/b/ref=dp_bc_6?ie=UTF8&amp;node=23658796011</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1265,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Protetora-Kicktok-Samsung-Celular-Transparente/dp/B0777RX2H3/ref=sr_1_10?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-10&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Protetora-Kicktok-Samsung-Celular-Transparente/dp/B0777RX2H3/ref=sr_1_10?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-10&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1144,7 +1294,11 @@
       <c r="I11" t="n">
         <v>4</v>
       </c>
-      <c r="J11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>681x1443</t>
+        </is>
+      </c>
       <c r="K11" t="b">
         <v>0</v>
       </c>
@@ -1155,7 +1309,22 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
+          <t>13146</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
           <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16244311011</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1341,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Pel%C3%ADcula-Protetora-Motorola-Celular-Transparente/dp/B075DZL4X6/ref=sr_1_11?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-11&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Pel%C3%ADcula-Protetora-Motorola-Celular-Transparente/dp/B075DZL4X6/ref=sr_1_11?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-11&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1216,7 +1385,22 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
+          <t>6667</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
           <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16244311011</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1417,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Pel%C3%ADcula-Protetora-Transparente-Motorola-Celular/dp/B07F6LKG2V/ref=sr_1_12?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-12&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Pel%C3%ADcula-Protetora-Transparente-Motorola-Celular/dp/B07F6LKG2V/ref=sr_1_12?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-12&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1277,55 +1461,70 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
+          <t>4976</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
           <t>https://www.amazon.com.br/Peliculas-Protetoras/b/ref=dp_bc_5?ie=UTF8&amp;node=16244091011</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Capa Protetora Cristal Bumper Transparente com Lateral Moto G7, Motorola, 4882.0, Preta</t>
+          <t>Capa Protetora Cristal Case Transparente Moto E5, Motorola, Capa com Proteção Completa (Carcaça+Tela), Transparente</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R$45,40</t>
+          <t>R$14,90</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Protetora-Cristal-Transparente-Motorola-4882-0/dp/B07NDB5ZD9/ref=sr_1_13?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-13&amp;ufe=app_do%3Aamzn1.fos.6d798eae-cadf-45de-946a-f477d47705b9&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Protetora-Transparente-Motorola-Prote%C3%A7%C3%A3o-Completa/dp/B07F7JXDVY/ref=sr_1_13?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-13&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Protege seu smartphone na parte traseira e laterais, com abertura para acessórios como carregadores e fones. Para o uso de outros acessórios não precisa retirar a capa. Evite riscos e impactos que podem danificar seu aparelho. Com acabamento refinado, dá maior aderência e segurança quando o aparelho está em suas mãos.</t>
+          <t>Protege seu smartphone na parte traseira e laterais. com abertura para acessórios como carregadores e fones. Para o uso de outros acessórios não precisa retirar a capa. Evite riscos e impactos que podem danificar seu aparelho.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>5 de 5</t>
+          <t>3,2 de 5</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['Para o uso de outros acessórios não precisa retirar a capa', 'Evite riscos e impactos que podem danificar seu aparelho.', 'Com acabamento refinado, dá maior aderência e segurança quando o aparelho está em suas mãos.', 'País de Origem: CN']</t>
+          <t>['Protege seu smartphone na parte traseira e laterais. com abertura para acessórios como carregadores e fones', 'Para o uso de outros acessórios não precisa retirar a capa', 'Evite riscos e impactos que podem danificar seu aparelho', 'País de Origem: CN']</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/615aJ73lEBL._AC_SL1500_.jpg</t>
+          <t>https://m.media-amazon.com/images/I/611KhH7BtTL._AC_SL1500_.jpg</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>638x1500</t>
+          <t>697x1433</t>
         </is>
       </c>
       <c r="K14" t="b">
@@ -1338,47 +1537,62 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
+          <t>7524</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
           <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16244311011</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Carregador Veicular Hightech, Energizer, EZ-DCA2CUWH3I, Branca</t>
+          <t>Capa Protetora Cristal Bumper Transparente com Lateral Moto G7, Motorola, 4882.0, Preta</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R$19,90</t>
+          <t>R$45,40</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Carregador-Veicular-Original-Energizer-Sa%C3%ADdas/dp/B0182JTL9G/ref=sr_1_14?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-14&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Protetora-Cristal-Transparente-Motorola-4882-0/dp/B07NDB5ZD9/ref=sr_1_14?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-14&amp;ufe=app_do%3Aamzn1.fos.6d798eae-cadf-45de-946a-f477d47705b9&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Carregue seus aparelhos enquanto está na rua ou na estrada. Com 3, 4 Amp potência de saída, este carregador Veicular Energizer com duas saídas USB, proporciona a carga rápida e segura de seus smartphones ou tablets.</t>
+          <t>Protege seu smartphone na parte traseira e laterais, com abertura para acessórios como carregadores e fones. Para o uso de outros acessórios não precisa retirar a capa. Evite riscos e impactos que podem danificar seu aparelho. Com acabamento refinado, dá maior aderência e segurança quando o aparelho está em suas mãos.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4,5 de 5</t>
+          <t>5 de 5</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['Carregue dois aparelhos simultaneamente', 'Obs: Não acompanha cabo USB', 'Design elegante']</t>
+          <t>['Para o uso de outros acessórios não precisa retirar a capa', 'Evite riscos e impactos que podem danificar seu aparelho.', 'Com acabamento refinado, dá maior aderência e segurança quando o aparelho está em suas mãos.', 'País de Origem: CN']</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/61t5kdNN+3L._AC_SL1500_.jpg</t>
+          <t>https://m.media-amazon.com/images/I/615aJ73lEBL._AC_SL1500_.jpg</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1386,7 +1600,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1160x1248</t>
+          <t>638x1500</t>
         </is>
       </c>
       <c r="K15" t="b">
@@ -1394,60 +1608,75 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Carregadores Veiculares</t>
+          <t>Capas Laterais</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Carregadores-Veiculares/b/ref=dp_bc_5?ie=UTF8&amp;node=16244303011</t>
+          <t>22483</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16244311011</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Capa Protetora Cristal Case Transparente Moto E5, Motorola, Capa com Proteção Completa (Carcaça+Tela), Transparente</t>
+          <t>Conj para Bar em Inox Stem 5 Pçs Prana Inox</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>R$14,90</t>
+          <t>R$199,90</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Protetora-Transparente-Motorola-Prote%C3%A7%C3%A3o-Completa/dp/B07F7JXDVY/ref=sr_1_15?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-15&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/CONJ-PARA-PRANA-Prana-000BS04008XXXNMS/dp/B07C1PYNZY/ref=sr_1_15?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-15&amp;ufe=app_do%3Aamzn1.fos.6121c6c4-c969-43ae-92f7-cc248fc6181d&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Protege seu smartphone na parte traseira e laterais. com abertura para acessórios como carregadores e fones. Para o uso de outros acessórios não precisa retirar a capa. Evite riscos e impactos que podem danificar seu aparelho.</t>
+          <t>Conj. Bar stem em aço inox no modelo liso. Contém peneira, faca, dosador, pinça. Todo feito em inox polido, deixa o lugar sofisticado como decoração e muito útil no preparo de drinks e bebidas com tudo o que é preciso para um preparo rápido.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3,2 de 5</t>
+          <t>Sem avaliação</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['Protege seu smartphone na parte traseira e laterais. com abertura para acessórios como carregadores e fones', 'Para o uso de outros acessórios não precisa retirar a capa', 'Evite riscos e impactos que podem danificar seu aparelho', 'País de Origem: CN']</t>
+          <t>['Com Design Limpo E Moderno, Trazendo Requinte E Sofisticação Para A Decoração De Seu Bar', 'Um Lindo Presente Para Homens Modernos Que Gostam De Preparar Seus Dinks Ou Receber Seus Convidados Com Elegncia', 'Em Aço Inox Polido, Prática De Limpar E Durável', 'País de Origem: CN']</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/611KhH7BtTL._AC_SL1500_.jpg</t>
+          <t>https://m.media-amazon.com/images/I/51n-vWG4HIL._AC_SL1000_.jpg</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>697x1433</t>
+          <t>611x893</t>
         </is>
       </c>
       <c r="K16" t="b">
@@ -1455,60 +1684,75 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Capas Laterais</t>
+          <t>Kits para Bar</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=16244311011</t>
+          <t>532</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/b/ref=dp_bc_4?ie=UTF8&amp;node=17125148011</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Conj para Bar em Inox Stem 5 Pçs Prana Inox</t>
+          <t>Carregador Veicular Hightech, Energizer, EZ-DCA2CUWH3I, Branca</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>R$199,90</t>
+          <t>R$19,90</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/CONJ-PARA-PRANA-Prana-000BS04008XXXNMS/dp/B07C1PYNZY/ref=sr_1_16?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQy4D6XkRe91SyzHh0aA3HqqAYh13TYtkf28luLUpqKdKYxdilEX4ZBI9cODJTEig0luYmtM4qnUstiXEQ2BqvBB1prwSJR7EozqV2Qy3YjTzFGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodm9igkYUVrFiq9hAyn5E-ktKeySD2f35RRaclvvMPpHz8PzuDy1Ck93AKfgPxw5WC4.FrqZ0joENNmRduDYE7-tNuS5qWPM63m8VQtvS0UiF_U&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748303&amp;s=merchant-items&amp;sr=1-16&amp;ufe=app_do%3Aamzn1.fos.6121c6c4-c969-43ae-92f7-cc248fc6181d&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Carregador-Veicular-Original-Energizer-Sa%C3%ADdas/dp/B0182JTL9G/ref=sr_1_16?dib=eyJ2IjoiMSJ9.an_1cY7E3LZNeVFRP4TQyz7_H4IYPNFkgGxEwby91AkKywokTOlb8c8SKWTmidMQySxXYjgIW_zxf9-tjXk7MPMZVY30GMRz8mmI4G4KkkrrgzByzMWpF5NtUA4A1GbvGj2xXOvznxaPCE_j3Fhst02QylxaUedF9OxRXxxUodmWq1v7F0_mvfeKst6WIkqLQAt0furxmrQjl4I1KCGhVsmIlF2fwcRAlVDBdXWXph0.xyzGpZQqjzPPzruWyiJkz3rESs-TLbTRHYcWmsH7v8c&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744891849&amp;s=merchant-items&amp;sr=1-16&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Conj. Bar stem em aço inox no modelo liso. Contém peneira, faca, dosador, pinça. Todo feito em inox polido, deixa o lugar sofisticado como decoração e muito útil no preparo de drinks e bebidas com tudo o que é preciso para um preparo rápido.</t>
+          <t>Carregue seus aparelhos enquanto está na rua ou na estrada. Com 3, 4 Amp potência de saída, este carregador Veicular Energizer com duas saídas USB, proporciona a carga rápida e segura de seus smartphones ou tablets.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Sem avaliação</t>
+          <t>4,5 de 5</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['Com Design Limpo E Moderno, Trazendo Requinte E Sofisticação Para A Decoração De Seu Bar', 'Um Lindo Presente Para Homens Modernos Que Gostam De Preparar Seus Dinks Ou Receber Seus Convidados Com Elegncia', 'Em Aço Inox Polido, Prática De Limpar E Durável', 'País de Origem: CN']</t>
+          <t>['Carregue dois aparelhos simultaneamente', 'Obs: Não acompanha cabo USB', 'Design elegante']</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/I/51n-vWG4HIL._AC_SL1000_.jpg</t>
+          <t>https://m.media-amazon.com/images/I/61t5kdNN+3L._AC_SL1500_.jpg</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>611x893</t>
+          <t>1160x1248</t>
         </is>
       </c>
       <c r="K17" t="b">
@@ -1516,12 +1760,27 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Kits para Bar</t>
+          <t>Carregadores Veiculares</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/b/ref=dp_bc_4?ie=UTF8&amp;node=17125148011</t>
+          <t>Indisponível</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Carregadores-Veiculares/b/ref=dp_bc_5?ie=UTF8&amp;node=16244303011</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>
@@ -1538,7 +1797,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Moldura-Dobravel-Plastica-Crismop-Inox/dp/B07GFW29QF/ref=sr_1_17?dib=eyJ2IjoiMSJ9.nJUGtznzO1_mp8QWZsUFXw.U2CihjVDI-ycq8hPBej8kXlvKnB5OP9svp036lzUguc&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744748834&amp;s=merchant-items&amp;sr=1-17&amp;xpid=tqkuqdh5H_SQg</t>
+          <t>https://www.amazon.com.br/Moldura-Dobravel-Plastica-Crismop-Inox/dp/B07GFW29QF/ref=sr_1_17?dib=eyJ2IjoiMSJ9.nJUGtznzO1_mp8QWZsUFXw.HAGC4Jy5KfIrmQLSJRa2tFfbjVfXS14L05fwjak5YJg&amp;dib_tag=se&amp;m=A2ZYQFB9FA7MU3&amp;marketplaceID=A2Q3Y263D00KWC&amp;qid=1744892216&amp;s=merchant-items&amp;sr=1-17&amp;xpid=tqkuqdh5H_SQg</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1582,7 +1841,22 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
+          <t>2719</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
           <t>https://www.amazon.com.br/b/ref=dp_bc_5?ie=UTF8&amp;node=17100787011</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>WayTechBr</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>17/04/2025</t>
         </is>
       </c>
     </row>

</xml_diff>